<commit_message>
ability to override titles
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -1320,10 +1320,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.19"/>
@@ -1368,7 +1368,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="245.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="245.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
support promo investigators (that need to be unhidden) support variant images in TTS (promo, revised investigators)
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="521">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -1445,6 +1445,144 @@
   </si>
   <si>
     <t xml:space="preserve">mini_investigators/60501b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hour of the Huntress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98001b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Dirge of Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tdor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98004b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norman Withers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98007a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ire of the Void</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iotv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98007b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolyn Fern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98010a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Fight the Black Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tftbw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98010b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silas Marsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98013a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Deep Gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tdg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98013b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dexter Drake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98016a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood of Baalshandor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98016b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m98019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gloria Goldberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98019a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark Revelations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/98019b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m99001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marie Lambeau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/05006a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/05006b.webp</t>
   </si>
 </sst>
 </file>
@@ -1549,12 +1687,12 @@
   <dimension ref="A1:AT1170"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+      <selection pane="bottomLeft" activeCell="A216" activeCellId="0" sqref="A216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.19"/>
@@ -13471,52 +13609,948 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1"/>
+      <c r="A201" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="D201" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E201" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G201" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="H201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I201" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="M201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S201" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS201" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1"/>
+      <c r="A202" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D202" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E202" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G202" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="H202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I202" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="M202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S202" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS202" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1"/>
+      <c r="A203" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="D203" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E203" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G203" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="H203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I203" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="M203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S203" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS203" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1"/>
+      <c r="A204" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C204" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D204" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E204" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G204" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="H204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I204" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="M204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S204" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS204" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="1"/>
+      <c r="A205" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D205" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E205" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G205" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="H205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I205" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="M205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S205" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS205" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1"/>
+      <c r="A206" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D206" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E206" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G206" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="H206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I206" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="M206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S206" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS206" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1"/>
+      <c r="A207" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="D207" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E207" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G207" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="H207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I207" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="M207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S207" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS207" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1"/>
+      <c r="A208" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B208" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D208" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E208" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G208" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="H208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I208" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="M208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S208" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS208" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="1"/>
+      <c r="A209" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D209" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E209" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G209" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="H209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I209" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="M209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S209" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS209" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="1"/>
+      <c r="A210" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="D210" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E210" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G210" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="H210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I210" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="M210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S210" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS210" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1"/>
+      <c r="A211" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="C211" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="D211" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E211" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G211" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="H211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I211" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="M211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S211" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS211" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="1"/>
+      <c r="A212" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="D212" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E212" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G212" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="H212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I212" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="M212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S212" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR212" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS212" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="1"/>
+      <c r="A213" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="D213" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E213" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G213" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="H213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I213" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="M213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S213" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR213" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS213" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="1"/>
+      <c r="A214" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D214" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E214" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G214" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="H214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I214" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="M214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S214" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR214" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS214" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="1"/>
+      <c r="A215" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B215" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C215" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="D215" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E215" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G215" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="H215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I215" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="M215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S215" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR215" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS215" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1"/>
+      <c r="A216" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B216" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C216" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="D216" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E216" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="G216" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="H216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I216" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="M216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S216" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR216" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS216" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1"/>

</xml_diff>

<commit_message>
changes about barrier (reverted)
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -2554,12 +2554,12 @@
   <dimension ref="A1:AT1375"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B164" activeCellId="0" sqref="B164"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.24"/>

</xml_diff>

<commit_message>
improved detection of player card backs detection of double-sided and linked at the same time ability to override full card data handle Dream-Eaters cards
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3393" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="847">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -2102,6 +2102,117 @@
   </si>
   <si>
     <t xml:space="preserve">micro_investigators/05049b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m06001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommy Muldoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Dream-Eaters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06001b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u06001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06001b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m06002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandy Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06002b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u06002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06002b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m06003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Morgan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06003b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u06003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06003b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m06004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luke Robinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06004b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u06004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06004b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m06005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patrice Hathaway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/06005b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u06005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/06005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">10016</t>
@@ -2551,7 +2662,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT1375"/>
+  <dimension ref="A1:AT1395"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2559,7 +2670,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.24"/>
@@ -2571,7 +2682,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.05"/>
@@ -24395,22 +24505,20 @@
         <v>58</v>
       </c>
       <c r="E369" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G369" s="0" t="s">
         <v>697</v>
       </c>
-      <c r="G369" s="0" t="s">
+      <c r="H369" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I369" s="0" t="s">
         <v>698</v>
       </c>
-      <c r="H369" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I369" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="J369" s="0" t="n">
-        <v>16</v>
-      </c>
+      <c r="J369" s="1"/>
       <c r="M369" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N369" s="0" t="n">
         <v>0</v>
@@ -24420,51 +24528,27 @@
       </c>
       <c r="P369" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="Q369" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="R369" s="0" t="s">
-        <v>701</v>
       </c>
       <c r="S369" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="V369" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="W369" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="X369" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y369" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA369" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="AB369" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AC369" s="0" t="n">
-        <v>6</v>
+      <c r="AL369" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="AP369" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ369" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR369" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS369" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="AT369" s="0" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24475,28 +24559,26 @@
         <v>695</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D370" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E370" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G370" s="0" t="s">
         <v>697</v>
       </c>
-      <c r="G370" s="0" t="s">
+      <c r="H370" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I370" s="0" t="s">
         <v>698</v>
       </c>
-      <c r="H370" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I370" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="J370" s="0" t="n">
-        <v>16</v>
-      </c>
+      <c r="J370" s="1"/>
       <c r="M370" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N370" s="0" t="n">
         <v>0</v>
@@ -24506,78 +24588,55 @@
       </c>
       <c r="P370" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="Q370" s="0" t="s">
-        <v>700</v>
-      </c>
-      <c r="R370" s="0" t="s">
-        <v>704</v>
       </c>
       <c r="S370" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="V370" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="W370" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X370" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y370" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA370" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="AB370" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AC370" s="0" t="n">
-        <v>4</v>
+      <c r="AL370" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="AP370" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ370" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR370" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS370" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="AT370" s="0" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="1" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="B371" s="0" t="s">
-        <v>707</v>
+        <v>695</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="D371" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E371" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G371" s="0" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="H371" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I371" s="0" t="s">
-        <v>709</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J371" s="1"/>
       <c r="M371" s="0" t="n">
         <v>0</v>
       </c>
@@ -24614,29 +24673,30 @@
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="1" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="B372" s="0" t="s">
-        <v>707</v>
+        <v>695</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="D372" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E372" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G372" s="0" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="H372" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I372" s="0" t="s">
-        <v>709</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J372" s="1"/>
       <c r="M372" s="0" t="n">
         <v>0</v>
       </c>
@@ -24673,29 +24733,30 @@
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="B373" s="0" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="D373" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E373" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G373" s="0" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="H373" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I373" s="0" t="s">
-        <v>709</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J373" s="1"/>
       <c r="M373" s="0" t="n">
         <v>0</v>
       </c>
@@ -24732,29 +24793,30 @@
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="1" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="B374" s="0" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="D374" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E374" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G374" s="0" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="H374" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I374" s="0" t="s">
-        <v>709</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J374" s="1"/>
       <c r="M374" s="0" t="n">
         <v>0</v>
       </c>
@@ -24791,29 +24853,30 @@
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="B375" s="0" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
       <c r="D375" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E375" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G375" s="0" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="H375" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I375" s="0" t="s">
-        <v>717</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J375" s="1"/>
       <c r="M375" s="0" t="n">
         <v>0</v>
       </c>
@@ -24850,29 +24913,30 @@
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="1" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>715</v>
+        <v>704</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="D376" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E376" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G376" s="0" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="H376" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I376" s="0" t="s">
-        <v>717</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J376" s="1"/>
       <c r="M376" s="0" t="n">
         <v>0</v>
       </c>
@@ -24909,29 +24973,30 @@
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="1" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="B377" s="0" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="D377" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E377" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G377" s="0" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="H377" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I377" s="0" t="s">
-        <v>717</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J377" s="1"/>
       <c r="M377" s="0" t="n">
         <v>0</v>
       </c>
@@ -24968,29 +25033,30 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="1" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="B378" s="0" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="D378" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E378" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G378" s="0" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="H378" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I378" s="0" t="s">
-        <v>717</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J378" s="1"/>
       <c r="M378" s="0" t="n">
         <v>0</v>
       </c>
@@ -25027,29 +25093,30 @@
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="1" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="B379" s="0" t="s">
-        <v>723</v>
+        <v>711</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="D379" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E379" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G379" s="0" t="s">
-        <v>723</v>
+        <v>697</v>
       </c>
       <c r="H379" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I379" s="0" t="s">
-        <v>725</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J379" s="1"/>
       <c r="M379" s="0" t="n">
         <v>0</v>
       </c>
@@ -25086,29 +25153,30 @@
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="1" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="B380" s="0" t="s">
-        <v>723</v>
+        <v>711</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>726</v>
+        <v>716</v>
       </c>
       <c r="D380" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E380" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G380" s="0" t="s">
-        <v>723</v>
+        <v>697</v>
       </c>
       <c r="H380" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I380" s="0" t="s">
-        <v>725</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J380" s="1"/>
       <c r="M380" s="0" t="n">
         <v>0</v>
       </c>
@@ -25145,29 +25213,30 @@
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
       <c r="B381" s="0" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="D381" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E381" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G381" s="0" t="s">
-        <v>723</v>
+        <v>697</v>
       </c>
       <c r="H381" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I381" s="0" t="s">
-        <v>725</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J381" s="1"/>
       <c r="M381" s="0" t="n">
         <v>0</v>
       </c>
@@ -25204,29 +25273,30 @@
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="1" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
       <c r="B382" s="0" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
       <c r="D382" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E382" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G382" s="0" t="s">
-        <v>723</v>
+        <v>697</v>
       </c>
       <c r="H382" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I382" s="0" t="s">
-        <v>725</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J382" s="1"/>
       <c r="M382" s="0" t="n">
         <v>0</v>
       </c>
@@ -25263,29 +25333,30 @@
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="1" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="B383" s="0" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="D383" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E383" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G383" s="0" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
       <c r="H383" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I383" s="0" t="s">
-        <v>733</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J383" s="1"/>
       <c r="M383" s="0" t="n">
         <v>0</v>
       </c>
@@ -25322,29 +25393,30 @@
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="B384" s="0" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
       <c r="D384" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E384" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G384" s="0" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
       <c r="H384" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I384" s="0" t="s">
-        <v>733</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J384" s="1"/>
       <c r="M384" s="0" t="n">
         <v>0</v>
       </c>
@@ -25381,29 +25453,30 @@
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="1" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
       <c r="B385" s="0" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
       <c r="D385" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E385" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G385" s="0" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
       <c r="H385" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I385" s="0" t="s">
-        <v>733</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J385" s="1"/>
       <c r="M385" s="0" t="n">
         <v>0</v>
       </c>
@@ -25440,29 +25513,30 @@
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="1" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
       <c r="B386" s="0" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
       <c r="D386" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E386" s="0" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G386" s="0" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
       <c r="H386" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I386" s="0" t="s">
-        <v>733</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J386" s="1"/>
       <c r="M386" s="0" t="n">
         <v>0</v>
       </c>
@@ -25499,29 +25573,30 @@
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="1" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="B387" s="0" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="D387" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E387" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G387" s="0" t="s">
-        <v>739</v>
+        <v>697</v>
       </c>
       <c r="H387" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I387" s="0" t="s">
-        <v>741</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J387" s="1"/>
       <c r="M387" s="0" t="n">
         <v>0</v>
       </c>
@@ -25558,29 +25633,30 @@
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="1" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="B388" s="0" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="C388" s="0" t="s">
-        <v>742</v>
+        <v>730</v>
       </c>
       <c r="D388" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E388" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G388" s="0" t="s">
-        <v>739</v>
+        <v>697</v>
       </c>
       <c r="H388" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I388" s="0" t="s">
-        <v>741</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="J388" s="1"/>
       <c r="M388" s="0" t="n">
         <v>0</v>
       </c>
@@ -25617,31 +25693,34 @@
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="1" t="s">
-        <v>743</v>
+        <v>731</v>
       </c>
       <c r="B389" s="0" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
       <c r="C389" s="0" t="s">
-        <v>744</v>
+        <v>733</v>
       </c>
       <c r="D389" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E389" s="0" t="s">
-        <v>448</v>
+        <v>734</v>
       </c>
       <c r="G389" s="0" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="H389" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I389" s="0" t="s">
-        <v>741</v>
+        <v>736</v>
+      </c>
+      <c r="J389" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="M389" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N389" s="0" t="n">
         <v>0</v>
@@ -25651,97 +25730,148 @@
       </c>
       <c r="P389" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="Q389" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="R389" s="0" t="s">
+        <v>738</v>
       </c>
       <c r="S389" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="V389" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W389" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="X389" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y389" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA389" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="AB389" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AL389" s="0" t="n">
-        <v>0</v>
+      <c r="AC389" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="AP389" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ389" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR389" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS389" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="AT389" s="0" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="1" t="s">
-        <v>743</v>
+        <v>731</v>
       </c>
       <c r="B390" s="0" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
       <c r="C390" s="0" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="D390" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E390" s="0" t="s">
-        <v>448</v>
+        <v>734</v>
       </c>
       <c r="G390" s="0" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="H390" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I390" s="0" t="s">
+        <v>736</v>
+      </c>
+      <c r="J390" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M390" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N390" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O390" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P390" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q390" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="R390" s="0" t="s">
         <v>741</v>
-      </c>
-      <c r="M390" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N390" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O390" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P390" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="S390" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="V390" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W390" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X390" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y390" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA390" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="AB390" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AL390" s="0" t="n">
-        <v>0</v>
+      <c r="AC390" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="AP390" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ390" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR390" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS390" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="AT390" s="0" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="1" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="B391" s="0" t="s">
-        <v>507</v>
+        <v>744</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D391" s="0" t="s">
         <v>58</v>
@@ -25750,13 +25880,13 @@
         <v>444</v>
       </c>
       <c r="G391" s="0" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="H391" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I391" s="0" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="M391" s="0" t="n">
         <v>0</v>
@@ -25794,13 +25924,13 @@
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="1" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="B392" s="0" t="s">
-        <v>507</v>
+        <v>744</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="D392" s="0" t="s">
         <v>58</v>
@@ -25809,13 +25939,13 @@
         <v>444</v>
       </c>
       <c r="G392" s="0" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="H392" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I392" s="0" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="M392" s="0" t="n">
         <v>0</v>
@@ -25853,13 +25983,13 @@
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="B393" s="0" t="s">
-        <v>507</v>
+        <v>744</v>
       </c>
       <c r="C393" s="0" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D393" s="0" t="s">
         <v>58</v>
@@ -25868,13 +25998,13 @@
         <v>448</v>
       </c>
       <c r="G393" s="0" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="H393" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I393" s="0" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="M393" s="0" t="n">
         <v>0</v>
@@ -25912,13 +26042,13 @@
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="B394" s="0" t="s">
-        <v>507</v>
+        <v>744</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="D394" s="0" t="s">
         <v>58</v>
@@ -25927,13 +26057,13 @@
         <v>448</v>
       </c>
       <c r="G394" s="0" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="H394" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I394" s="0" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="M394" s="0" t="n">
         <v>0</v>
@@ -25971,13 +26101,13 @@
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="1" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="B395" s="0" t="s">
-        <v>442</v>
+        <v>752</v>
       </c>
       <c r="C395" s="0" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D395" s="0" t="s">
         <v>58</v>
@@ -25986,13 +26116,13 @@
         <v>444</v>
       </c>
       <c r="G395" s="0" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="H395" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I395" s="0" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="M395" s="0" t="n">
         <v>0</v>
@@ -26030,13 +26160,13 @@
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="B396" s="0" t="s">
-        <v>442</v>
+        <v>752</v>
       </c>
       <c r="C396" s="0" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D396" s="0" t="s">
         <v>58</v>
@@ -26045,13 +26175,13 @@
         <v>444</v>
       </c>
       <c r="G396" s="0" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="H396" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I396" s="0" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="M396" s="0" t="n">
         <v>0</v>
@@ -26089,13 +26219,13 @@
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B397" s="0" t="s">
-        <v>442</v>
+        <v>752</v>
       </c>
       <c r="C397" s="0" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D397" s="0" t="s">
         <v>58</v>
@@ -26104,13 +26234,13 @@
         <v>448</v>
       </c>
       <c r="G397" s="0" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="H397" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I397" s="0" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="M397" s="0" t="n">
         <v>0</v>
@@ -26148,13 +26278,13 @@
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B398" s="0" t="s">
-        <v>442</v>
+        <v>752</v>
       </c>
       <c r="C398" s="0" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D398" s="0" t="s">
         <v>58</v>
@@ -26163,13 +26293,13 @@
         <v>448</v>
       </c>
       <c r="G398" s="0" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="H398" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I398" s="0" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="M398" s="0" t="n">
         <v>0</v>
@@ -26207,13 +26337,13 @@
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B399" s="0" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="C399" s="0" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D399" s="0" t="s">
         <v>58</v>
@@ -26222,13 +26352,13 @@
         <v>444</v>
       </c>
       <c r="G399" s="0" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="H399" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I399" s="0" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="M399" s="0" t="n">
         <v>0</v>
@@ -26266,13 +26396,13 @@
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B400" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="C400" s="0" t="s">
         <v>763</v>
-      </c>
-      <c r="C400" s="0" t="s">
-        <v>767</v>
       </c>
       <c r="D400" s="0" t="s">
         <v>58</v>
@@ -26281,13 +26411,13 @@
         <v>444</v>
       </c>
       <c r="G400" s="0" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="H400" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I400" s="0" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="M400" s="0" t="n">
         <v>0</v>
@@ -26325,13 +26455,13 @@
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="B401" s="0" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="C401" s="0" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D401" s="0" t="s">
         <v>58</v>
@@ -26340,13 +26470,13 @@
         <v>448</v>
       </c>
       <c r="G401" s="0" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="H401" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I401" s="0" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="M401" s="0" t="n">
         <v>0</v>
@@ -26384,13 +26514,13 @@
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="B402" s="0" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="C402" s="0" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="D402" s="0" t="s">
         <v>58</v>
@@ -26399,13 +26529,13 @@
         <v>448</v>
       </c>
       <c r="G402" s="0" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="H402" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I402" s="0" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="M402" s="0" t="n">
         <v>0</v>
@@ -26443,13 +26573,13 @@
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="B403" s="0" t="s">
-        <v>623</v>
+        <v>768</v>
       </c>
       <c r="C403" s="0" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D403" s="0" t="s">
         <v>58</v>
@@ -26458,13 +26588,13 @@
         <v>444</v>
       </c>
       <c r="G403" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="H403" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I403" s="0" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="M403" s="0" t="n">
         <v>0</v>
@@ -26502,13 +26632,13 @@
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B404" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="C404" s="0" t="s">
         <v>771</v>
-      </c>
-      <c r="B404" s="0" t="s">
-        <v>623</v>
-      </c>
-      <c r="C404" s="0" t="s">
-        <v>775</v>
       </c>
       <c r="D404" s="0" t="s">
         <v>58</v>
@@ -26517,13 +26647,13 @@
         <v>444</v>
       </c>
       <c r="G404" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="H404" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I404" s="0" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="M404" s="0" t="n">
         <v>0</v>
@@ -26561,13 +26691,13 @@
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="1" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="B405" s="0" t="s">
-        <v>623</v>
+        <v>768</v>
       </c>
       <c r="C405" s="0" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D405" s="0" t="s">
         <v>58</v>
@@ -26576,13 +26706,13 @@
         <v>448</v>
       </c>
       <c r="G405" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="H405" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I405" s="0" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="M405" s="0" t="n">
         <v>0</v>
@@ -26620,13 +26750,13 @@
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="1" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="B406" s="0" t="s">
-        <v>623</v>
+        <v>768</v>
       </c>
       <c r="C406" s="0" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D406" s="0" t="s">
         <v>58</v>
@@ -26635,13 +26765,13 @@
         <v>448</v>
       </c>
       <c r="G406" s="0" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="H406" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I406" s="0" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="M406" s="0" t="n">
         <v>0</v>
@@ -26679,13 +26809,13 @@
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="1" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B407" s="0" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C407" s="0" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D407" s="0" t="s">
         <v>58</v>
@@ -26694,13 +26824,13 @@
         <v>444</v>
       </c>
       <c r="G407" s="0" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="H407" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I407" s="0" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="M407" s="0" t="n">
         <v>0</v>
@@ -26738,13 +26868,13 @@
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B408" s="0" t="s">
+        <v>776</v>
+      </c>
+      <c r="C408" s="0" t="s">
         <v>779</v>
-      </c>
-      <c r="B408" s="0" t="s">
-        <v>780</v>
-      </c>
-      <c r="C408" s="0" t="s">
-        <v>784</v>
       </c>
       <c r="D408" s="0" t="s">
         <v>58</v>
@@ -26753,13 +26883,13 @@
         <v>444</v>
       </c>
       <c r="G408" s="0" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="H408" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I408" s="0" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="M408" s="0" t="n">
         <v>0</v>
@@ -26797,13 +26927,13 @@
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="1" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="B409" s="0" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C409" s="0" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="D409" s="0" t="s">
         <v>58</v>
@@ -26812,13 +26942,13 @@
         <v>448</v>
       </c>
       <c r="G409" s="0" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="H409" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I409" s="0" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="M409" s="0" t="n">
         <v>0</v>
@@ -26856,13 +26986,13 @@
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="1" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="B410" s="0" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C410" s="0" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="D410" s="0" t="s">
         <v>58</v>
@@ -26871,13 +27001,13 @@
         <v>448</v>
       </c>
       <c r="G410" s="0" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="H410" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I410" s="0" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="M410" s="0" t="n">
         <v>0</v>
@@ -26915,13 +27045,13 @@
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="1" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="B411" s="0" t="s">
-        <v>789</v>
+        <v>507</v>
       </c>
       <c r="C411" s="0" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="D411" s="0" t="s">
         <v>58</v>
@@ -26930,13 +27060,13 @@
         <v>444</v>
       </c>
       <c r="G411" s="0" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="H411" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I411" s="0" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="M411" s="0" t="n">
         <v>0</v>
@@ -26974,13 +27104,13 @@
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="1" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="B412" s="0" t="s">
-        <v>789</v>
+        <v>507</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="D412" s="0" t="s">
         <v>58</v>
@@ -26989,13 +27119,13 @@
         <v>444</v>
       </c>
       <c r="G412" s="0" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="H412" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I412" s="0" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="M412" s="0" t="n">
         <v>0</v>
@@ -27033,13 +27163,13 @@
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="1" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="B413" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="C413" s="0" t="s">
         <v>789</v>
-      </c>
-      <c r="C413" s="0" t="s">
-        <v>795</v>
       </c>
       <c r="D413" s="0" t="s">
         <v>58</v>
@@ -27048,13 +27178,13 @@
         <v>448</v>
       </c>
       <c r="G413" s="0" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="H413" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I413" s="0" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="M413" s="0" t="n">
         <v>0</v>
@@ -27092,13 +27222,13 @@
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="1" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="B414" s="0" t="s">
-        <v>789</v>
+        <v>507</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="D414" s="0" t="s">
         <v>58</v>
@@ -27107,13 +27237,13 @@
         <v>448</v>
       </c>
       <c r="G414" s="0" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="H414" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I414" s="0" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="M414" s="0" t="n">
         <v>0</v>
@@ -27151,13 +27281,13 @@
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="1" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="B415" s="0" t="s">
-        <v>798</v>
+        <v>442</v>
       </c>
       <c r="C415" s="0" t="s">
-        <v>799</v>
+        <v>792</v>
       </c>
       <c r="D415" s="0" t="s">
         <v>58</v>
@@ -27166,13 +27296,13 @@
         <v>444</v>
       </c>
       <c r="G415" s="0" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="H415" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I415" s="0" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="M415" s="0" t="n">
         <v>0</v>
@@ -27210,13 +27340,13 @@
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="1" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>798</v>
+        <v>442</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="D416" s="0" t="s">
         <v>58</v>
@@ -27225,13 +27355,13 @@
         <v>444</v>
       </c>
       <c r="G416" s="0" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="H416" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I416" s="0" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="M416" s="0" t="n">
         <v>0</v>
@@ -27269,13 +27399,13 @@
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="1" t="s">
-        <v>803</v>
+        <v>796</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>798</v>
+        <v>442</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="D417" s="0" t="s">
         <v>58</v>
@@ -27284,13 +27414,13 @@
         <v>448</v>
       </c>
       <c r="G417" s="0" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="H417" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I417" s="0" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="M417" s="0" t="n">
         <v>0</v>
@@ -27328,13 +27458,13 @@
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="1" t="s">
-        <v>803</v>
+        <v>796</v>
       </c>
       <c r="B418" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="C418" s="0" t="s">
         <v>798</v>
-      </c>
-      <c r="C418" s="0" t="s">
-        <v>805</v>
       </c>
       <c r="D418" s="0" t="s">
         <v>58</v>
@@ -27343,13 +27473,13 @@
         <v>448</v>
       </c>
       <c r="G418" s="0" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="H418" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I418" s="0" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="M418" s="0" t="n">
         <v>0</v>
@@ -27387,13 +27517,13 @@
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="1" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="B419" s="0" t="s">
-        <v>660</v>
+        <v>800</v>
       </c>
       <c r="C419" s="0" t="s">
-        <v>661</v>
+        <v>801</v>
       </c>
       <c r="D419" s="0" t="s">
         <v>58</v>
@@ -27402,13 +27532,13 @@
         <v>444</v>
       </c>
       <c r="G419" s="0" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="H419" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I419" s="0" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="M419" s="0" t="n">
         <v>0</v>
@@ -27446,13 +27576,13 @@
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>660</v>
+        <v>800</v>
       </c>
       <c r="C420" s="0" t="s">
-        <v>662</v>
+        <v>804</v>
       </c>
       <c r="D420" s="0" t="s">
         <v>58</v>
@@ -27461,13 +27591,13 @@
         <v>444</v>
       </c>
       <c r="G420" s="0" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="H420" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I420" s="0" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="M420" s="0" t="n">
         <v>0</v>
@@ -27505,13 +27635,13 @@
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>660</v>
+        <v>800</v>
       </c>
       <c r="C421" s="0" t="s">
-        <v>664</v>
+        <v>806</v>
       </c>
       <c r="D421" s="0" t="s">
         <v>58</v>
@@ -27520,13 +27650,13 @@
         <v>448</v>
       </c>
       <c r="G421" s="0" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="H421" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I421" s="0" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="M421" s="0" t="n">
         <v>0</v>
@@ -27564,13 +27694,13 @@
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>660</v>
+        <v>800</v>
       </c>
       <c r="C422" s="0" t="s">
-        <v>665</v>
+        <v>807</v>
       </c>
       <c r="D422" s="0" t="s">
         <v>58</v>
@@ -27579,13 +27709,13 @@
         <v>448</v>
       </c>
       <c r="G422" s="0" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="H422" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I422" s="0" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="M422" s="0" t="n">
         <v>0</v>
@@ -27621,65 +27751,1185 @@
         <v>0</v>
       </c>
     </row>
-    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A521" s="1"/>
-    </row>
-    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A522" s="1"/>
-    </row>
-    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="1"/>
-    </row>
-    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A524" s="1"/>
-    </row>
-    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A525" s="1"/>
-    </row>
-    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="1"/>
-    </row>
-    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="1"/>
-    </row>
-    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A528" s="1"/>
-    </row>
-    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A529" s="1"/>
-    </row>
-    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="1"/>
-    </row>
-    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A531" s="1"/>
-    </row>
-    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="1"/>
-    </row>
-    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A533" s="1"/>
-    </row>
-    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A534" s="1"/>
-    </row>
-    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A535" s="1"/>
-    </row>
-    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A536" s="1"/>
-    </row>
-    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="1"/>
-    </row>
-    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A538" s="1"/>
-    </row>
-    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A539" s="1"/>
-    </row>
-    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A540" s="1"/>
+    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C423" s="0" t="s">
+        <v>809</v>
+      </c>
+      <c r="D423" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E423" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G423" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="H423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I423" s="0" t="s">
+        <v>811</v>
+      </c>
+      <c r="M423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S423" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR423" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS423" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B424" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C424" s="0" t="s">
+        <v>812</v>
+      </c>
+      <c r="D424" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E424" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G424" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="H424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I424" s="0" t="s">
+        <v>811</v>
+      </c>
+      <c r="M424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S424" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR424" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS424" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B425" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C425" s="0" t="s">
+        <v>814</v>
+      </c>
+      <c r="D425" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E425" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G425" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="H425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I425" s="0" t="s">
+        <v>811</v>
+      </c>
+      <c r="M425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S425" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR425" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS425" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B426" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C426" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="D426" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E426" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G426" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="H426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I426" s="0" t="s">
+        <v>811</v>
+      </c>
+      <c r="M426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S426" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR426" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS426" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B427" s="0" t="s">
+        <v>817</v>
+      </c>
+      <c r="C427" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="D427" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E427" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G427" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="H427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I427" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="M427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S427" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR427" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS427" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B428" s="0" t="s">
+        <v>817</v>
+      </c>
+      <c r="C428" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="D428" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E428" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G428" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="H428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I428" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="M428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S428" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS428" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B429" s="0" t="s">
+        <v>817</v>
+      </c>
+      <c r="C429" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="D429" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E429" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G429" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="H429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I429" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="M429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S429" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR429" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS429" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B430" s="0" t="s">
+        <v>817</v>
+      </c>
+      <c r="C430" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="D430" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E430" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G430" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="H430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I430" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="M430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S430" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR430" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS430" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B431" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C431" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="D431" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E431" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G431" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="H431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I431" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="M431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S431" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS431" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B432" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C432" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="D432" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E432" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G432" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="H432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I432" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="M432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S432" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS432" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C433" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="D433" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E433" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G433" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="H433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I433" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="M433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S433" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS433" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B434" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C434" s="0" t="s">
+        <v>833</v>
+      </c>
+      <c r="D434" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E434" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G434" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="H434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I434" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="M434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S434" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS434" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B435" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="C435" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="D435" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E435" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G435" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="H435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I435" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="M435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S435" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS435" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B436" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="C436" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="D436" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E436" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G436" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="H436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I436" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="M436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S436" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS436" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B437" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="C437" s="0" t="s">
+        <v>841</v>
+      </c>
+      <c r="D437" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E437" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G437" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="H437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I437" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="M437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S437" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS437" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B438" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="C438" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="D438" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E438" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G438" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="H438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I438" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="M438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S438" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS438" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B439" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C439" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="D439" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E439" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G439" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="H439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I439" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="M439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S439" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR439" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS439" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B440" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C440" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="D440" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E440" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G440" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="H440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I440" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="M440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S440" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR440" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS440" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B441" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C441" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="D441" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E441" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G441" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="H441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I441" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="M441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S441" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR441" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS441" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B442" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C442" s="0" t="s">
+        <v>665</v>
+      </c>
+      <c r="D442" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E442" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G442" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="H442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I442" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="M442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S442" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR442" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS442" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="1"/>
@@ -29697,6 +30947,24 @@
     <row r="1212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1212" s="1"/>
     </row>
+    <row r="1213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1213" s="1"/>
+    </row>
+    <row r="1214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1214" s="1"/>
+    </row>
+    <row r="1215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1215" s="1"/>
+    </row>
+    <row r="1216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1216" s="1"/>
+    </row>
+    <row r="1217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1217" s="1"/>
+    </row>
+    <row r="1218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1218" s="1"/>
+    </row>
     <row r="1219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1219" s="1"/>
     </row>
@@ -29739,24 +31007,6 @@
     <row r="1232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1232" s="1"/>
     </row>
-    <row r="1233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1233" s="1"/>
-    </row>
-    <row r="1234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1234" s="1"/>
-    </row>
-    <row r="1235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1235" s="1"/>
-    </row>
-    <row r="1236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1236" s="1"/>
-    </row>
-    <row r="1237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1237" s="1"/>
-    </row>
-    <row r="1238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1238" s="1"/>
-    </row>
     <row r="1239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1239" s="1"/>
     </row>
@@ -29793,6 +31043,36 @@
     <row r="1250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1250" s="1"/>
     </row>
+    <row r="1251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1251" s="1"/>
+    </row>
+    <row r="1252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1252" s="1"/>
+    </row>
+    <row r="1253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1253" s="1"/>
+    </row>
+    <row r="1254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1254" s="1"/>
+    </row>
+    <row r="1255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1255" s="1"/>
+    </row>
+    <row r="1256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1256" s="1"/>
+    </row>
+    <row r="1257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1257" s="1"/>
+    </row>
+    <row r="1258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1258" s="1"/>
+    </row>
+    <row r="1259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1259" s="1"/>
+    </row>
+    <row r="1260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1260" s="1"/>
+    </row>
     <row r="1261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1261" s="1"/>
     </row>
@@ -29823,30 +31103,6 @@
     <row r="1270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1270" s="1"/>
     </row>
-    <row r="1271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1271" s="1"/>
-    </row>
-    <row r="1272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1272" s="1"/>
-    </row>
-    <row r="1275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1275" s="1"/>
-    </row>
-    <row r="1276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1276" s="1"/>
-    </row>
-    <row r="1277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1277" s="1"/>
-    </row>
-    <row r="1278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1278" s="1"/>
-    </row>
-    <row r="1279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1279" s="1"/>
-    </row>
-    <row r="1280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1280" s="1"/>
-    </row>
     <row r="1281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1281" s="1"/>
     </row>
@@ -29862,6 +31118,18 @@
     <row r="1285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1285" s="1"/>
     </row>
+    <row r="1286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1286" s="1"/>
+    </row>
+    <row r="1287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1287" s="1"/>
+    </row>
+    <row r="1288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1288" s="1"/>
+    </row>
+    <row r="1289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1289" s="1"/>
+    </row>
     <row r="1290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1290" s="1"/>
     </row>
@@ -29871,12 +31139,6 @@
     <row r="1292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1292" s="1"/>
     </row>
-    <row r="1293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1293" s="1"/>
-    </row>
-    <row r="1294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1294" s="1"/>
-    </row>
     <row r="1295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1295" s="1"/>
     </row>
@@ -29910,18 +31172,6 @@
     <row r="1305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1305" s="1"/>
     </row>
-    <row r="1306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1306" s="1"/>
-    </row>
-    <row r="1307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1307" s="1"/>
-    </row>
-    <row r="1308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1308" s="1"/>
-    </row>
-    <row r="1309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1309" s="1"/>
-    </row>
     <row r="1310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1310" s="1"/>
     </row>
@@ -30119,6 +31369,66 @@
     </row>
     <row r="1375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1375" s="1"/>
+    </row>
+    <row r="1376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1376" s="1"/>
+    </row>
+    <row r="1377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1377" s="1"/>
+    </row>
+    <row r="1378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1378" s="1"/>
+    </row>
+    <row r="1379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1379" s="1"/>
+    </row>
+    <row r="1380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1380" s="1"/>
+    </row>
+    <row r="1381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1381" s="1"/>
+    </row>
+    <row r="1382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1382" s="1"/>
+    </row>
+    <row r="1383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1383" s="1"/>
+    </row>
+    <row r="1384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1384" s="1"/>
+    </row>
+    <row r="1385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1385" s="1"/>
+    </row>
+    <row r="1386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1386" s="1"/>
+    </row>
+    <row r="1387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1387" s="1"/>
+    </row>
+    <row r="1388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1388" s="1"/>
+    </row>
+    <row r="1389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1389" s="1"/>
+    </row>
+    <row r="1390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1390" s="1"/>
+    </row>
+    <row r="1391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1391" s="1"/>
+    </row>
+    <row r="1392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1392" s="1"/>
+    </row>
+    <row r="1393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1393" s="1"/>
+    </row>
+    <row r="1394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1394" s="1"/>
+    </row>
+    <row r="1395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1395" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
support all parallel investigators
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3553" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="864">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -2369,6 +2369,189 @@
   </si>
   <si>
     <t xml:space="preserve">micro_investigators/60501b.webp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">08007</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Monterey Jack</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mini_investigators/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">08007</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">a.webp</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Edge of the Earth Investigator Expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eoep</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mini_investigators/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">08007</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b.webp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">08007</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">micro_investigators/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">08007</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">a.webp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">micro_investigators/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">08007</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b.webp</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">m90084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/90084a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pistols and Pearls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/90084b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u90084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/90084a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/90084b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98001</t>
@@ -2571,7 +2754,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2592,6 +2775,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2636,12 +2824,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2662,15 +2854,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT1395"/>
+  <dimension ref="A1:AT1403"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A376" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A411" activeCellId="0" sqref="A411"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.24"/>
@@ -27047,11 +27239,11 @@
       <c r="A411" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="B411" s="0" t="s">
-        <v>507</v>
+      <c r="B411" s="2" t="s">
+        <v>784</v>
       </c>
       <c r="C411" s="0" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D411" s="0" t="s">
         <v>58</v>
@@ -27059,14 +27251,14 @@
       <c r="E411" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="G411" s="0" t="s">
-        <v>785</v>
+      <c r="G411" s="2" t="s">
+        <v>786</v>
       </c>
       <c r="H411" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I411" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="M411" s="0" t="n">
         <v>0</v>
@@ -27106,11 +27298,11 @@
       <c r="A412" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="B412" s="0" t="s">
-        <v>507</v>
+      <c r="B412" s="2" t="s">
+        <v>784</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D412" s="0" t="s">
         <v>58</v>
@@ -27118,14 +27310,14 @@
       <c r="E412" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="G412" s="0" t="s">
-        <v>785</v>
+      <c r="G412" s="2" t="s">
+        <v>786</v>
       </c>
       <c r="H412" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I412" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="M412" s="0" t="n">
         <v>0</v>
@@ -27163,13 +27355,13 @@
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="B413" s="0" t="s">
-        <v>507</v>
+        <v>789</v>
+      </c>
+      <c r="B413" s="2" t="s">
+        <v>784</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D413" s="0" t="s">
         <v>58</v>
@@ -27177,14 +27369,14 @@
       <c r="E413" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="G413" s="0" t="s">
-        <v>785</v>
+      <c r="G413" s="2" t="s">
+        <v>786</v>
       </c>
       <c r="H413" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I413" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="M413" s="0" t="n">
         <v>0</v>
@@ -27222,13 +27414,13 @@
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="B414" s="0" t="s">
-        <v>507</v>
+        <v>789</v>
+      </c>
+      <c r="B414" s="2" t="s">
+        <v>784</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D414" s="0" t="s">
         <v>58</v>
@@ -27236,14 +27428,14 @@
       <c r="E414" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="G414" s="0" t="s">
-        <v>785</v>
+      <c r="G414" s="2" t="s">
+        <v>786</v>
       </c>
       <c r="H414" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I414" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="M414" s="0" t="n">
         <v>0</v>
@@ -27281,13 +27473,13 @@
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B415" s="0" t="s">
-        <v>442</v>
+        <v>507</v>
       </c>
       <c r="C415" s="0" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D415" s="0" t="s">
         <v>58</v>
@@ -27296,13 +27488,13 @@
         <v>444</v>
       </c>
       <c r="G415" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="H415" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I415" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M415" s="0" t="n">
         <v>0</v>
@@ -27340,13 +27532,13 @@
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>442</v>
+        <v>507</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D416" s="0" t="s">
         <v>58</v>
@@ -27355,13 +27547,13 @@
         <v>444</v>
       </c>
       <c r="G416" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="H416" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I416" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M416" s="0" t="n">
         <v>0</v>
@@ -27399,13 +27591,13 @@
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>442</v>
+        <v>507</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D417" s="0" t="s">
         <v>58</v>
@@ -27414,13 +27606,13 @@
         <v>448</v>
       </c>
       <c r="G417" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="H417" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I417" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M417" s="0" t="n">
         <v>0</v>
@@ -27458,13 +27650,13 @@
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B418" s="0" t="s">
-        <v>442</v>
+        <v>507</v>
       </c>
       <c r="C418" s="0" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="D418" s="0" t="s">
         <v>58</v>
@@ -27473,13 +27665,13 @@
         <v>448</v>
       </c>
       <c r="G418" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="H418" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I418" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M418" s="0" t="n">
         <v>0</v>
@@ -27517,10 +27709,10 @@
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B419" s="0" t="s">
-        <v>800</v>
+        <v>507</v>
       </c>
       <c r="C419" s="0" t="s">
         <v>801</v>
@@ -27576,10 +27768,10 @@
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>800</v>
+        <v>507</v>
       </c>
       <c r="C420" s="0" t="s">
         <v>804</v>
@@ -27638,7 +27830,7 @@
         <v>805</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>800</v>
+        <v>507</v>
       </c>
       <c r="C421" s="0" t="s">
         <v>806</v>
@@ -27697,7 +27889,7 @@
         <v>805</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>800</v>
+        <v>507</v>
       </c>
       <c r="C422" s="0" t="s">
         <v>807</v>
@@ -27756,7 +27948,7 @@
         <v>808</v>
       </c>
       <c r="B423" s="0" t="s">
-        <v>623</v>
+        <v>442</v>
       </c>
       <c r="C423" s="0" t="s">
         <v>809</v>
@@ -27815,7 +28007,7 @@
         <v>808</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>623</v>
+        <v>442</v>
       </c>
       <c r="C424" s="0" t="s">
         <v>812</v>
@@ -27874,7 +28066,7 @@
         <v>813</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>623</v>
+        <v>442</v>
       </c>
       <c r="C425" s="0" t="s">
         <v>814</v>
@@ -27933,7 +28125,7 @@
         <v>813</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>623</v>
+        <v>442</v>
       </c>
       <c r="C426" s="0" t="s">
         <v>815</v>
@@ -28228,10 +28420,10 @@
         <v>825</v>
       </c>
       <c r="B431" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C431" s="0" t="s">
         <v>826</v>
-      </c>
-      <c r="C431" s="0" t="s">
-        <v>827</v>
       </c>
       <c r="D431" s="0" t="s">
         <v>58</v>
@@ -28240,13 +28432,13 @@
         <v>444</v>
       </c>
       <c r="G431" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="H431" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I431" s="0" t="s">
         <v>828</v>
-      </c>
-      <c r="H431" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I431" s="0" t="s">
-        <v>829</v>
       </c>
       <c r="M431" s="0" t="n">
         <v>0</v>
@@ -28287,10 +28479,10 @@
         <v>825</v>
       </c>
       <c r="B432" s="0" t="s">
-        <v>826</v>
+        <v>623</v>
       </c>
       <c r="C432" s="0" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D432" s="0" t="s">
         <v>58</v>
@@ -28299,13 +28491,13 @@
         <v>444</v>
       </c>
       <c r="G432" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="H432" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I432" s="0" t="s">
         <v>828</v>
-      </c>
-      <c r="H432" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I432" s="0" t="s">
-        <v>829</v>
       </c>
       <c r="M432" s="0" t="n">
         <v>0</v>
@@ -28343,13 +28535,13 @@
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="C433" s="0" t="s">
         <v>831</v>
-      </c>
-      <c r="B433" s="0" t="s">
-        <v>826</v>
-      </c>
-      <c r="C433" s="0" t="s">
-        <v>832</v>
       </c>
       <c r="D433" s="0" t="s">
         <v>58</v>
@@ -28358,13 +28550,13 @@
         <v>448</v>
       </c>
       <c r="G433" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="H433" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I433" s="0" t="s">
         <v>828</v>
-      </c>
-      <c r="H433" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I433" s="0" t="s">
-        <v>829</v>
       </c>
       <c r="M433" s="0" t="n">
         <v>0</v>
@@ -28402,13 +28594,13 @@
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B434" s="0" t="s">
-        <v>826</v>
+        <v>623</v>
       </c>
       <c r="C434" s="0" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D434" s="0" t="s">
         <v>58</v>
@@ -28417,13 +28609,13 @@
         <v>448</v>
       </c>
       <c r="G434" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="H434" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I434" s="0" t="s">
         <v>828</v>
-      </c>
-      <c r="H434" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I434" s="0" t="s">
-        <v>829</v>
       </c>
       <c r="M434" s="0" t="n">
         <v>0</v>
@@ -28461,13 +28653,13 @@
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B435" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="B435" s="0" t="s">
+      <c r="C435" s="0" t="s">
         <v>835</v>
-      </c>
-      <c r="C435" s="0" t="s">
-        <v>836</v>
       </c>
       <c r="D435" s="0" t="s">
         <v>58</v>
@@ -28476,13 +28668,13 @@
         <v>444</v>
       </c>
       <c r="G435" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="H435" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I435" s="0" t="s">
         <v>837</v>
-      </c>
-      <c r="H435" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I435" s="0" t="s">
-        <v>838</v>
       </c>
       <c r="M435" s="0" t="n">
         <v>0</v>
@@ -28520,13 +28712,13 @@
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B436" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="B436" s="0" t="s">
-        <v>835</v>
-      </c>
       <c r="C436" s="0" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D436" s="0" t="s">
         <v>58</v>
@@ -28535,13 +28727,13 @@
         <v>444</v>
       </c>
       <c r="G436" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="H436" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I436" s="0" t="s">
         <v>837</v>
-      </c>
-      <c r="H436" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I436" s="0" t="s">
-        <v>838</v>
       </c>
       <c r="M436" s="0" t="n">
         <v>0</v>
@@ -28579,13 +28771,13 @@
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="B437" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="C437" s="0" t="s">
         <v>840</v>
-      </c>
-      <c r="B437" s="0" t="s">
-        <v>835</v>
-      </c>
-      <c r="C437" s="0" t="s">
-        <v>841</v>
       </c>
       <c r="D437" s="0" t="s">
         <v>58</v>
@@ -28594,13 +28786,13 @@
         <v>448</v>
       </c>
       <c r="G437" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="H437" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I437" s="0" t="s">
         <v>837</v>
-      </c>
-      <c r="H437" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I437" s="0" t="s">
-        <v>838</v>
       </c>
       <c r="M437" s="0" t="n">
         <v>0</v>
@@ -28638,13 +28830,13 @@
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B438" s="0" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C438" s="0" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D438" s="0" t="s">
         <v>58</v>
@@ -28653,13 +28845,13 @@
         <v>448</v>
       </c>
       <c r="G438" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="H438" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I438" s="0" t="s">
         <v>837</v>
-      </c>
-      <c r="H438" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I438" s="0" t="s">
-        <v>838</v>
       </c>
       <c r="M438" s="0" t="n">
         <v>0</v>
@@ -28697,13 +28889,13 @@
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B439" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="B439" s="0" t="s">
-        <v>660</v>
-      </c>
       <c r="C439" s="0" t="s">
-        <v>661</v>
+        <v>844</v>
       </c>
       <c r="D439" s="0" t="s">
         <v>58</v>
@@ -28712,13 +28904,13 @@
         <v>444</v>
       </c>
       <c r="G439" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H439" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I439" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="M439" s="0" t="n">
         <v>0</v>
@@ -28756,13 +28948,13 @@
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B440" s="0" t="s">
         <v>843</v>
       </c>
-      <c r="B440" s="0" t="s">
-        <v>660</v>
-      </c>
       <c r="C440" s="0" t="s">
-        <v>662</v>
+        <v>847</v>
       </c>
       <c r="D440" s="0" t="s">
         <v>58</v>
@@ -28771,13 +28963,13 @@
         <v>444</v>
       </c>
       <c r="G440" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H440" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I440" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="M440" s="0" t="n">
         <v>0</v>
@@ -28815,13 +29007,13 @@
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B441" s="0" t="s">
-        <v>660</v>
+        <v>843</v>
       </c>
       <c r="C441" s="0" t="s">
-        <v>664</v>
+        <v>849</v>
       </c>
       <c r="D441" s="0" t="s">
         <v>58</v>
@@ -28830,13 +29022,13 @@
         <v>448</v>
       </c>
       <c r="G441" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H441" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I441" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="M441" s="0" t="n">
         <v>0</v>
@@ -28874,13 +29066,13 @@
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B442" s="0" t="s">
-        <v>660</v>
+        <v>843</v>
       </c>
       <c r="C442" s="0" t="s">
-        <v>665</v>
+        <v>850</v>
       </c>
       <c r="D442" s="0" t="s">
         <v>58</v>
@@ -28889,13 +29081,13 @@
         <v>448</v>
       </c>
       <c r="G442" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H442" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I442" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="M442" s="0" t="n">
         <v>0</v>
@@ -28931,29 +29123,477 @@
         <v>0</v>
       </c>
     </row>
-    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A541" s="1"/>
-    </row>
-    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A542" s="1"/>
-    </row>
-    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A543" s="1"/>
-    </row>
-    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A544" s="1"/>
-    </row>
-    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A545" s="1"/>
-    </row>
-    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A546" s="1"/>
-    </row>
-    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A547" s="1"/>
-    </row>
-    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A548" s="1"/>
+    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B443" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="C443" s="0" t="s">
+        <v>853</v>
+      </c>
+      <c r="D443" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E443" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G443" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="H443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I443" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="M443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S443" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR443" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS443" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B444" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="C444" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="D444" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E444" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G444" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="H444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I444" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="M444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S444" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR444" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS444" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B445" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="C445" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="D445" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E445" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G445" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="H445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I445" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="M445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S445" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR445" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS445" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A446" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B446" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="C446" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="D446" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E446" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G446" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="H446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I446" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="M446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S446" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR446" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS446" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B447" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C447" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="D447" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E447" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G447" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="H447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I447" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="M447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S447" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR447" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS447" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B448" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C448" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="D448" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E448" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="G448" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="H448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I448" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="M448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S448" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR448" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS448" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B449" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C449" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="D449" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E449" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G449" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="H449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I449" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="M449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S449" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR449" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS449" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A450" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B450" s="0" t="s">
+        <v>660</v>
+      </c>
+      <c r="C450" s="0" t="s">
+        <v>665</v>
+      </c>
+      <c r="D450" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E450" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="G450" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="H450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I450" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="M450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S450" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR450" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS450" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="1"/>
@@ -31007,30 +31647,30 @@
     <row r="1232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1232" s="1"/>
     </row>
+    <row r="1233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1233" s="1"/>
+    </row>
+    <row r="1234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1234" s="1"/>
+    </row>
+    <row r="1235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1235" s="1"/>
+    </row>
+    <row r="1236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1236" s="1"/>
+    </row>
+    <row r="1237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1237" s="1"/>
+    </row>
+    <row r="1238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1238" s="1"/>
+    </row>
     <row r="1239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1239" s="1"/>
     </row>
     <row r="1240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1240" s="1"/>
     </row>
-    <row r="1241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1241" s="1"/>
-    </row>
-    <row r="1242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1242" s="1"/>
-    </row>
-    <row r="1243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1243" s="1"/>
-    </row>
-    <row r="1244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1244" s="1"/>
-    </row>
-    <row r="1245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1245" s="1"/>
-    </row>
-    <row r="1246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1246" s="1"/>
-    </row>
     <row r="1247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1247" s="1"/>
     </row>
@@ -31103,29 +31743,29 @@
     <row r="1270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1270" s="1"/>
     </row>
-    <row r="1281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1281" s="1"/>
-    </row>
-    <row r="1282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1282" s="1"/>
-    </row>
-    <row r="1283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1283" s="1"/>
-    </row>
-    <row r="1284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1284" s="1"/>
-    </row>
-    <row r="1285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1285" s="1"/>
-    </row>
-    <row r="1286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1286" s="1"/>
-    </row>
-    <row r="1287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1287" s="1"/>
-    </row>
-    <row r="1288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1288" s="1"/>
+    <row r="1271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1271" s="1"/>
+    </row>
+    <row r="1272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1272" s="1"/>
+    </row>
+    <row r="1273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1273" s="1"/>
+    </row>
+    <row r="1274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1274" s="1"/>
+    </row>
+    <row r="1275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1275" s="1"/>
+    </row>
+    <row r="1276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1276" s="1"/>
+    </row>
+    <row r="1277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1277" s="1"/>
+    </row>
+    <row r="1278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1278" s="1"/>
     </row>
     <row r="1289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1289" s="1"/>
@@ -31139,6 +31779,12 @@
     <row r="1292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1292" s="1"/>
     </row>
+    <row r="1293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1293" s="1"/>
+    </row>
+    <row r="1294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1294" s="1"/>
+    </row>
     <row r="1295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1295" s="1"/>
     </row>
@@ -31157,12 +31803,6 @@
     <row r="1300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1300" s="1"/>
     </row>
-    <row r="1301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1301" s="1"/>
-    </row>
-    <row r="1302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1302" s="1"/>
-    </row>
     <row r="1303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1303" s="1"/>
     </row>
@@ -31172,6 +31812,18 @@
     <row r="1305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1305" s="1"/>
     </row>
+    <row r="1306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1306" s="1"/>
+    </row>
+    <row r="1307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1307" s="1"/>
+    </row>
+    <row r="1308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1308" s="1"/>
+    </row>
+    <row r="1309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1309" s="1"/>
+    </row>
     <row r="1310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1310" s="1"/>
     </row>
@@ -31184,18 +31836,6 @@
     <row r="1313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1313" s="1"/>
     </row>
-    <row r="1314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1314" s="1"/>
-    </row>
-    <row r="1315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1315" s="1"/>
-    </row>
-    <row r="1316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1316" s="1"/>
-    </row>
-    <row r="1317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1317" s="1"/>
-    </row>
     <row r="1318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1318" s="1"/>
     </row>
@@ -31429,6 +32069,30 @@
     </row>
     <row r="1395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1395" s="1"/>
+    </row>
+    <row r="1396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1396" s="1"/>
+    </row>
+    <row r="1397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1397" s="1"/>
+    </row>
+    <row r="1398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1398" s="1"/>
+    </row>
+    <row r="1399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1399" s="1"/>
+    </row>
+    <row r="1400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1400" s="1"/>
+    </row>
+    <row r="1401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1401" s="1"/>
+    </row>
+    <row r="1402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1402" s="1"/>
+    </row>
+    <row r="1403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1403" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
TIC cards, parallel Mateo some improvements and fixes
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3761" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3921" uniqueCount="941">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -2347,6 +2347,111 @@
     <t xml:space="preserve">micro_investigators/06005b.webp</t>
   </si>
   <si>
+    <t xml:space="preserve">m07001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sister Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07001b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u07001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07001b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m07002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amanda Sharpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07002b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u07002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07002b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m07003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trish Scarborough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07003b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u07003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07003b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m07004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dexter Drake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07004b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u07004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07004b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m07005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silas Marsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini_investigators/07005b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u07005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micro_investigators/07005b.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">10016</t>
   </si>
   <si>
@@ -2656,9 +2761,6 @@
     <t xml:space="preserve">m98013</t>
   </si>
   <si>
-    <t xml:space="preserve">Silas Marsh</t>
-  </si>
-  <si>
     <t xml:space="preserve">mini_investigators/98013a.webp</t>
   </si>
   <si>
@@ -2681,9 +2783,6 @@
   </si>
   <si>
     <t xml:space="preserve">m98016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dexter Drake</t>
   </si>
   <si>
     <t xml:space="preserve">mini_investigators/98016a.webp</t>
@@ -2754,7 +2853,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2775,11 +2874,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2824,16 +2918,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2858,15 +2948,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT1421"/>
+  <dimension ref="A1:AT1441"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A390" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A426" activeCellId="0" sqref="A426"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.24"/>
@@ -5596,7 +5686,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B45" s="0" t="s">
@@ -5655,7 +5745,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B46" s="0" t="s">
@@ -5714,7 +5804,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B47" s="0" t="s">
@@ -5773,7 +5863,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B48" s="0" t="s">
@@ -26963,22 +27053,20 @@
         <v>58</v>
       </c>
       <c r="E407" s="0" t="s">
-        <v>778</v>
+        <v>488</v>
       </c>
       <c r="G407" s="0" t="s">
-        <v>779</v>
+        <v>110</v>
       </c>
       <c r="H407" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I407" s="0" t="s">
-        <v>780</v>
-      </c>
-      <c r="J407" s="0" t="n">
-        <v>16</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J407" s="1"/>
       <c r="M407" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N407" s="0" t="n">
         <v>0</v>
@@ -26988,51 +27076,27 @@
       </c>
       <c r="P407" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="Q407" s="0" t="s">
-        <v>781</v>
-      </c>
-      <c r="R407" s="0" t="s">
-        <v>782</v>
       </c>
       <c r="S407" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="V407" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="W407" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="X407" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="Y407" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA407" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="AB407" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AC407" s="0" t="n">
-        <v>6</v>
+      <c r="AL407" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="AP407" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ407" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR407" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS407" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="AT407" s="0" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27043,28 +27107,26 @@
         <v>776</v>
       </c>
       <c r="C408" s="0" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="D408" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E408" s="0" t="s">
-        <v>778</v>
+        <v>488</v>
       </c>
       <c r="G408" s="0" t="s">
-        <v>779</v>
+        <v>110</v>
       </c>
       <c r="H408" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I408" s="0" t="s">
-        <v>780</v>
-      </c>
-      <c r="J408" s="0" t="n">
-        <v>16</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J408" s="1"/>
       <c r="M408" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N408" s="0" t="n">
         <v>0</v>
@@ -27074,78 +27136,55 @@
       </c>
       <c r="P408" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="Q408" s="0" t="s">
-        <v>781</v>
-      </c>
-      <c r="R408" s="0" t="s">
-        <v>785</v>
       </c>
       <c r="S408" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="V408" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="W408" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X408" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="Y408" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA408" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="AB408" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AC408" s="0" t="n">
-        <v>4</v>
+      <c r="AL408" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="AP408" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ408" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR408" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS408" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="AT408" s="0" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="1" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="B409" s="0" t="s">
-        <v>788</v>
+        <v>776</v>
       </c>
       <c r="C409" s="0" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="D409" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E409" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G409" s="0" t="s">
-        <v>788</v>
+        <v>110</v>
       </c>
       <c r="H409" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I409" s="0" t="s">
-        <v>790</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J409" s="1"/>
       <c r="M409" s="0" t="n">
         <v>0</v>
       </c>
@@ -27182,29 +27221,30 @@
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="1" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="B410" s="0" t="s">
-        <v>788</v>
+        <v>776</v>
       </c>
       <c r="C410" s="0" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
       <c r="D410" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E410" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G410" s="0" t="s">
-        <v>788</v>
+        <v>110</v>
       </c>
       <c r="H410" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I410" s="0" t="s">
-        <v>790</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J410" s="1"/>
       <c r="M410" s="0" t="n">
         <v>0</v>
       </c>
@@ -27241,29 +27281,30 @@
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="1" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="B411" s="0" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="C411" s="0" t="s">
-        <v>793</v>
+        <v>784</v>
       </c>
       <c r="D411" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E411" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G411" s="0" t="s">
-        <v>788</v>
+        <v>110</v>
       </c>
       <c r="H411" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I411" s="0" t="s">
-        <v>790</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J411" s="1"/>
       <c r="M411" s="0" t="n">
         <v>0</v>
       </c>
@@ -27300,29 +27341,30 @@
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="1" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="B412" s="0" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>794</v>
+        <v>785</v>
       </c>
       <c r="D412" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E412" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G412" s="0" t="s">
-        <v>788</v>
+        <v>110</v>
       </c>
       <c r="H412" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I412" s="0" t="s">
-        <v>790</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J412" s="1"/>
       <c r="M412" s="0" t="n">
         <v>0</v>
       </c>
@@ -27359,29 +27401,30 @@
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="1" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="B413" s="0" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="C413" s="0" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="D413" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E413" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G413" s="0" t="s">
-        <v>796</v>
+        <v>110</v>
       </c>
       <c r="H413" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I413" s="0" t="s">
-        <v>798</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J413" s="1"/>
       <c r="M413" s="0" t="n">
         <v>0</v>
       </c>
@@ -27418,29 +27461,30 @@
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="1" t="s">
-        <v>795</v>
+        <v>786</v>
       </c>
       <c r="B414" s="0" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="C414" s="0" t="s">
-        <v>799</v>
+        <v>788</v>
       </c>
       <c r="D414" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E414" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G414" s="0" t="s">
-        <v>796</v>
+        <v>110</v>
       </c>
       <c r="H414" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I414" s="0" t="s">
-        <v>798</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J414" s="1"/>
       <c r="M414" s="0" t="n">
         <v>0</v>
       </c>
@@ -27477,29 +27521,30 @@
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="1" t="s">
-        <v>800</v>
+        <v>789</v>
       </c>
       <c r="B415" s="0" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="C415" s="0" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="D415" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E415" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G415" s="0" t="s">
-        <v>796</v>
+        <v>110</v>
       </c>
       <c r="H415" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I415" s="0" t="s">
-        <v>798</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J415" s="1"/>
       <c r="M415" s="0" t="n">
         <v>0</v>
       </c>
@@ -27536,29 +27581,30 @@
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="1" t="s">
-        <v>800</v>
+        <v>789</v>
       </c>
       <c r="B416" s="0" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="C416" s="0" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
       <c r="D416" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E416" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G416" s="0" t="s">
-        <v>796</v>
+        <v>110</v>
       </c>
       <c r="H416" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I416" s="0" t="s">
-        <v>798</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J416" s="1"/>
       <c r="M416" s="0" t="n">
         <v>0</v>
       </c>
@@ -27595,29 +27641,30 @@
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="1" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="B417" s="0" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="C417" s="0" t="s">
-        <v>805</v>
+        <v>794</v>
       </c>
       <c r="D417" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E417" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G417" s="0" t="s">
-        <v>804</v>
+        <v>110</v>
       </c>
       <c r="H417" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I417" s="0" t="s">
-        <v>806</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J417" s="1"/>
       <c r="M417" s="0" t="n">
         <v>0</v>
       </c>
@@ -27654,29 +27701,30 @@
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="1" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="B418" s="0" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="C418" s="0" t="s">
-        <v>807</v>
+        <v>795</v>
       </c>
       <c r="D418" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E418" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G418" s="0" t="s">
-        <v>804</v>
+        <v>110</v>
       </c>
       <c r="H418" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I418" s="0" t="s">
-        <v>806</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J418" s="1"/>
       <c r="M418" s="0" t="n">
         <v>0</v>
       </c>
@@ -27713,29 +27761,30 @@
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="1" t="s">
-        <v>808</v>
+        <v>796</v>
       </c>
       <c r="B419" s="0" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="C419" s="0" t="s">
-        <v>809</v>
+        <v>798</v>
       </c>
       <c r="D419" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E419" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G419" s="0" t="s">
-        <v>804</v>
+        <v>110</v>
       </c>
       <c r="H419" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I419" s="0" t="s">
-        <v>806</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J419" s="1"/>
       <c r="M419" s="0" t="n">
         <v>0</v>
       </c>
@@ -27772,29 +27821,30 @@
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="s">
-        <v>808</v>
+        <v>796</v>
       </c>
       <c r="B420" s="0" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="C420" s="0" t="s">
-        <v>810</v>
+        <v>799</v>
       </c>
       <c r="D420" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E420" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G420" s="0" t="s">
-        <v>804</v>
+        <v>110</v>
       </c>
       <c r="H420" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I420" s="0" t="s">
-        <v>806</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J420" s="1"/>
       <c r="M420" s="0" t="n">
         <v>0</v>
       </c>
@@ -27831,29 +27881,30 @@
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="s">
-        <v>811</v>
+        <v>800</v>
       </c>
       <c r="B421" s="0" t="s">
-        <v>812</v>
+        <v>797</v>
       </c>
       <c r="C421" s="0" t="s">
-        <v>813</v>
+        <v>801</v>
       </c>
       <c r="D421" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E421" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G421" s="0" t="s">
-        <v>812</v>
+        <v>110</v>
       </c>
       <c r="H421" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I421" s="0" t="s">
-        <v>814</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J421" s="1"/>
       <c r="M421" s="0" t="n">
         <v>0</v>
       </c>
@@ -27890,29 +27941,30 @@
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
-        <v>811</v>
+        <v>800</v>
       </c>
       <c r="B422" s="0" t="s">
-        <v>812</v>
+        <v>797</v>
       </c>
       <c r="C422" s="0" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="D422" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E422" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G422" s="0" t="s">
-        <v>812</v>
+        <v>110</v>
       </c>
       <c r="H422" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I422" s="0" t="s">
-        <v>814</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J422" s="1"/>
       <c r="M422" s="0" t="n">
         <v>0</v>
       </c>
@@ -27949,29 +28001,30 @@
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="1" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="B423" s="0" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="C423" s="0" t="s">
-        <v>817</v>
+        <v>805</v>
       </c>
       <c r="D423" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E423" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G423" s="0" t="s">
-        <v>812</v>
+        <v>110</v>
       </c>
       <c r="H423" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I423" s="0" t="s">
-        <v>814</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J423" s="1"/>
       <c r="M423" s="0" t="n">
         <v>0</v>
       </c>
@@ -28008,29 +28061,30 @@
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="1" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="B424" s="0" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="C424" s="0" t="s">
-        <v>818</v>
+        <v>806</v>
       </c>
       <c r="D424" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E424" s="0" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G424" s="0" t="s">
-        <v>812</v>
+        <v>110</v>
       </c>
       <c r="H424" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I424" s="0" t="s">
-        <v>814</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J424" s="1"/>
       <c r="M424" s="0" t="n">
         <v>0</v>
       </c>
@@ -28067,29 +28121,30 @@
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="s">
-        <v>819</v>
+        <v>807</v>
       </c>
       <c r="B425" s="0" t="s">
-        <v>820</v>
+        <v>804</v>
       </c>
       <c r="C425" s="0" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="D425" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E425" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G425" s="0" t="s">
-        <v>820</v>
+        <v>110</v>
       </c>
       <c r="H425" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I425" s="0" t="s">
-        <v>822</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J425" s="1"/>
       <c r="M425" s="0" t="n">
         <v>0</v>
       </c>
@@ -28126,29 +28181,30 @@
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="s">
-        <v>819</v>
+        <v>807</v>
       </c>
       <c r="B426" s="0" t="s">
-        <v>820</v>
+        <v>804</v>
       </c>
       <c r="C426" s="0" t="s">
-        <v>823</v>
+        <v>809</v>
       </c>
       <c r="D426" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E426" s="0" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="G426" s="0" t="s">
-        <v>820</v>
+        <v>110</v>
       </c>
       <c r="H426" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I426" s="0" t="s">
-        <v>822</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="J426" s="1"/>
       <c r="M426" s="0" t="n">
         <v>0</v>
       </c>
@@ -28185,31 +28241,34 @@
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="s">
-        <v>824</v>
+        <v>810</v>
       </c>
       <c r="B427" s="0" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="C427" s="0" t="s">
-        <v>825</v>
+        <v>812</v>
       </c>
       <c r="D427" s="0" t="s">
         <v>58</v>
       </c>
       <c r="E427" s="0" t="s">
-        <v>492</v>
+        <v>813</v>
       </c>
       <c r="G427" s="0" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="H427" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I427" s="0" t="s">
-        <v>822</v>
+        <v>815</v>
+      </c>
+      <c r="J427" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="M427" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N427" s="0" t="n">
         <v>0</v>
@@ -28219,97 +28278,148 @@
       </c>
       <c r="P427" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="Q427" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="R427" s="0" t="s">
+        <v>817</v>
       </c>
       <c r="S427" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="V427" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="W427" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="X427" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y427" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA427" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="AB427" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AL427" s="0" t="n">
-        <v>0</v>
+      <c r="AC427" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="AP427" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ427" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR427" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS427" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="AT427" s="0" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="s">
-        <v>824</v>
+        <v>810</v>
       </c>
       <c r="B428" s="0" t="s">
+        <v>811</v>
+      </c>
+      <c r="C428" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="D428" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E428" s="0" t="s">
+        <v>813</v>
+      </c>
+      <c r="G428" s="0" t="s">
+        <v>814</v>
+      </c>
+      <c r="H428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I428" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="J428" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M428" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P428" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q428" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="R428" s="0" t="s">
         <v>820</v>
-      </c>
-      <c r="C428" s="0" t="s">
-        <v>826</v>
-      </c>
-      <c r="D428" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E428" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="G428" s="0" t="s">
-        <v>820</v>
-      </c>
-      <c r="H428" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I428" s="0" t="s">
-        <v>822</v>
-      </c>
-      <c r="M428" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N428" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O428" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P428" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="S428" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="V428" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="W428" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X428" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y428" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA428" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="AB428" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AL428" s="0" t="n">
-        <v>0</v>
+      <c r="AC428" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="AP428" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AQ428" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR428" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AS428" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="AT428" s="0" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="B429" s="3" t="s">
-        <v>828</v>
+        <v>822</v>
+      </c>
+      <c r="B429" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="C429" s="0" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="D429" s="0" t="s">
         <v>58</v>
@@ -28317,14 +28427,14 @@
       <c r="E429" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="G429" s="3" t="s">
-        <v>830</v>
+      <c r="G429" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="H429" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I429" s="0" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="M429" s="0" t="n">
         <v>0</v>
@@ -28362,13 +28472,13 @@
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="B430" s="3" t="s">
-        <v>828</v>
+        <v>822</v>
+      </c>
+      <c r="B430" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="C430" s="0" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="D430" s="0" t="s">
         <v>58</v>
@@ -28376,14 +28486,14 @@
       <c r="E430" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="G430" s="3" t="s">
-        <v>830</v>
+      <c r="G430" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="H430" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I430" s="0" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="M430" s="0" t="n">
         <v>0</v>
@@ -28421,13 +28531,13 @@
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="B431" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="B431" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="C431" s="0" t="s">
         <v>828</v>
-      </c>
-      <c r="C431" s="0" t="s">
-        <v>834</v>
       </c>
       <c r="D431" s="0" t="s">
         <v>58</v>
@@ -28435,14 +28545,14 @@
       <c r="E431" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="G431" s="3" t="s">
-        <v>830</v>
+      <c r="G431" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="H431" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I431" s="0" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="M431" s="0" t="n">
         <v>0</v>
@@ -28480,13 +28590,13 @@
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="B432" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
+      </c>
+      <c r="B432" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="C432" s="0" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="D432" s="0" t="s">
         <v>58</v>
@@ -28494,14 +28604,14 @@
       <c r="E432" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="G432" s="3" t="s">
-        <v>830</v>
+      <c r="G432" s="0" t="s">
+        <v>823</v>
       </c>
       <c r="H432" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I432" s="0" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="M432" s="0" t="n">
         <v>0</v>
@@ -28539,13 +28649,13 @@
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="B433" s="0" t="s">
-        <v>551</v>
+        <v>831</v>
       </c>
       <c r="C433" s="0" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="D433" s="0" t="s">
         <v>58</v>
@@ -28554,13 +28664,13 @@
         <v>488</v>
       </c>
       <c r="G433" s="0" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="H433" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I433" s="0" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="M433" s="0" t="n">
         <v>0</v>
@@ -28598,13 +28708,13 @@
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="B434" s="0" t="s">
-        <v>551</v>
+        <v>831</v>
       </c>
       <c r="C434" s="0" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="D434" s="0" t="s">
         <v>58</v>
@@ -28613,13 +28723,13 @@
         <v>488</v>
       </c>
       <c r="G434" s="0" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="H434" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I434" s="0" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="M434" s="0" t="n">
         <v>0</v>
@@ -28657,13 +28767,13 @@
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="B435" s="0" t="s">
-        <v>551</v>
+        <v>831</v>
       </c>
       <c r="C435" s="0" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="D435" s="0" t="s">
         <v>58</v>
@@ -28672,13 +28782,13 @@
         <v>492</v>
       </c>
       <c r="G435" s="0" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="H435" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I435" s="0" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="M435" s="0" t="n">
         <v>0</v>
@@ -28716,13 +28826,13 @@
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="B436" s="0" t="s">
-        <v>551</v>
+        <v>831</v>
       </c>
       <c r="C436" s="0" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="D436" s="0" t="s">
         <v>58</v>
@@ -28731,13 +28841,13 @@
         <v>492</v>
       </c>
       <c r="G436" s="0" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="H436" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I436" s="0" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="M436" s="0" t="n">
         <v>0</v>
@@ -28775,13 +28885,13 @@
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B437" s="0" t="s">
-        <v>551</v>
+        <v>839</v>
       </c>
       <c r="C437" s="0" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="D437" s="0" t="s">
         <v>58</v>
@@ -28790,13 +28900,13 @@
         <v>488</v>
       </c>
       <c r="G437" s="0" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="H437" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I437" s="0" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="M437" s="0" t="n">
         <v>0</v>
@@ -28834,13 +28944,13 @@
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B438" s="0" t="s">
-        <v>551</v>
+        <v>839</v>
       </c>
       <c r="C438" s="0" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="D438" s="0" t="s">
         <v>58</v>
@@ -28849,13 +28959,13 @@
         <v>488</v>
       </c>
       <c r="G438" s="0" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="H438" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I438" s="0" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="M438" s="0" t="n">
         <v>0</v>
@@ -28893,13 +29003,13 @@
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="B439" s="0" t="s">
-        <v>551</v>
+        <v>839</v>
       </c>
       <c r="C439" s="0" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="D439" s="0" t="s">
         <v>58</v>
@@ -28908,13 +29018,13 @@
         <v>492</v>
       </c>
       <c r="G439" s="0" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="H439" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I439" s="0" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="M439" s="0" t="n">
         <v>0</v>
@@ -28952,13 +29062,13 @@
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="B440" s="0" t="s">
-        <v>551</v>
+        <v>839</v>
       </c>
       <c r="C440" s="0" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="D440" s="0" t="s">
         <v>58</v>
@@ -28967,13 +29077,13 @@
         <v>492</v>
       </c>
       <c r="G440" s="0" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="H440" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I440" s="0" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="M440" s="0" t="n">
         <v>0</v>
@@ -29011,13 +29121,13 @@
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="B441" s="0" t="s">
-        <v>486</v>
+        <v>847</v>
       </c>
       <c r="C441" s="0" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="D441" s="0" t="s">
         <v>58</v>
@@ -29026,13 +29136,13 @@
         <v>488</v>
       </c>
       <c r="G441" s="0" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="H441" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I441" s="0" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="M441" s="0" t="n">
         <v>0</v>
@@ -29070,13 +29180,13 @@
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="B442" s="0" t="s">
-        <v>486</v>
+        <v>847</v>
       </c>
       <c r="C442" s="0" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="D442" s="0" t="s">
         <v>58</v>
@@ -29085,13 +29195,13 @@
         <v>488</v>
       </c>
       <c r="G442" s="0" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="H442" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I442" s="0" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="M442" s="0" t="n">
         <v>0</v>
@@ -29129,13 +29239,13 @@
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="1" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="B443" s="0" t="s">
-        <v>486</v>
+        <v>847</v>
       </c>
       <c r="C443" s="0" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="D443" s="0" t="s">
         <v>58</v>
@@ -29144,13 +29254,13 @@
         <v>492</v>
       </c>
       <c r="G443" s="0" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="H443" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I443" s="0" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="M443" s="0" t="n">
         <v>0</v>
@@ -29188,13 +29298,13 @@
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="B444" s="0" t="s">
-        <v>486</v>
+        <v>847</v>
       </c>
       <c r="C444" s="0" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="D444" s="0" t="s">
         <v>58</v>
@@ -29203,13 +29313,13 @@
         <v>492</v>
       </c>
       <c r="G444" s="0" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="H444" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I444" s="0" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="M444" s="0" t="n">
         <v>0</v>
@@ -29247,13 +29357,13 @@
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="1" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="B445" s="0" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="C445" s="0" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="D445" s="0" t="s">
         <v>58</v>
@@ -29262,13 +29372,13 @@
         <v>488</v>
       </c>
       <c r="G445" s="0" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="H445" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I445" s="0" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="M445" s="0" t="n">
         <v>0</v>
@@ -29306,13 +29416,13 @@
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="1" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="B446" s="0" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="C446" s="0" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
       <c r="D446" s="0" t="s">
         <v>58</v>
@@ -29321,13 +29431,13 @@
         <v>488</v>
       </c>
       <c r="G446" s="0" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="H446" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I446" s="0" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="M446" s="0" t="n">
         <v>0</v>
@@ -29365,13 +29475,13 @@
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="1" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="B447" s="0" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="C447" s="0" t="s">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="D447" s="0" t="s">
         <v>58</v>
@@ -29380,13 +29490,13 @@
         <v>492</v>
       </c>
       <c r="G447" s="0" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="H447" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I447" s="0" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="M447" s="0" t="n">
         <v>0</v>
@@ -29424,13 +29534,13 @@
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="1" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="B448" s="0" t="s">
+        <v>855</v>
+      </c>
+      <c r="C448" s="0" t="s">
         <v>861</v>
-      </c>
-      <c r="C448" s="0" t="s">
-        <v>868</v>
       </c>
       <c r="D448" s="0" t="s">
         <v>58</v>
@@ -29439,13 +29549,13 @@
         <v>492</v>
       </c>
       <c r="G448" s="0" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="H448" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I448" s="0" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="M448" s="0" t="n">
         <v>0</v>
@@ -29483,13 +29593,13 @@
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="1" t="s">
-        <v>869</v>
-      </c>
-      <c r="B449" s="0" t="s">
-        <v>667</v>
+        <v>862</v>
+      </c>
+      <c r="B449" s="2" t="s">
+        <v>863</v>
       </c>
       <c r="C449" s="0" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="D449" s="0" t="s">
         <v>58</v>
@@ -29497,14 +29607,14 @@
       <c r="E449" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="G449" s="0" t="s">
-        <v>871</v>
+      <c r="G449" s="2" t="s">
+        <v>865</v>
       </c>
       <c r="H449" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I449" s="0" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="M449" s="0" t="n">
         <v>0</v>
@@ -29542,13 +29652,13 @@
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="1" t="s">
-        <v>869</v>
-      </c>
-      <c r="B450" s="0" t="s">
-        <v>667</v>
+        <v>862</v>
+      </c>
+      <c r="B450" s="2" t="s">
+        <v>863</v>
       </c>
       <c r="C450" s="0" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="D450" s="0" t="s">
         <v>58</v>
@@ -29556,14 +29666,14 @@
       <c r="E450" s="0" t="s">
         <v>488</v>
       </c>
-      <c r="G450" s="0" t="s">
-        <v>871</v>
+      <c r="G450" s="2" t="s">
+        <v>865</v>
       </c>
       <c r="H450" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I450" s="0" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="M450" s="0" t="n">
         <v>0</v>
@@ -29601,13 +29711,13 @@
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="B451" s="0" t="s">
-        <v>667</v>
+        <v>868</v>
+      </c>
+      <c r="B451" s="2" t="s">
+        <v>863</v>
       </c>
       <c r="C451" s="0" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="D451" s="0" t="s">
         <v>58</v>
@@ -29615,14 +29725,14 @@
       <c r="E451" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="G451" s="0" t="s">
-        <v>871</v>
+      <c r="G451" s="2" t="s">
+        <v>865</v>
       </c>
       <c r="H451" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I451" s="0" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="M451" s="0" t="n">
         <v>0</v>
@@ -29660,13 +29770,13 @@
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="B452" s="0" t="s">
-        <v>667</v>
+        <v>868</v>
+      </c>
+      <c r="B452" s="2" t="s">
+        <v>863</v>
       </c>
       <c r="C452" s="0" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="D452" s="0" t="s">
         <v>58</v>
@@ -29674,14 +29784,14 @@
       <c r="E452" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="G452" s="0" t="s">
-        <v>871</v>
+      <c r="G452" s="2" t="s">
+        <v>865</v>
       </c>
       <c r="H452" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I452" s="0" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="M452" s="0" t="n">
         <v>0</v>
@@ -29719,13 +29829,13 @@
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="1" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="B453" s="0" t="s">
-        <v>878</v>
+        <v>551</v>
       </c>
       <c r="C453" s="0" t="s">
-        <v>879</v>
+        <v>872</v>
       </c>
       <c r="D453" s="0" t="s">
         <v>58</v>
@@ -29734,13 +29844,13 @@
         <v>488</v>
       </c>
       <c r="G453" s="0" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="H453" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I453" s="0" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="M453" s="0" t="n">
         <v>0</v>
@@ -29778,13 +29888,13 @@
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="1" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="B454" s="0" t="s">
-        <v>878</v>
+        <v>551</v>
       </c>
       <c r="C454" s="0" t="s">
-        <v>882</v>
+        <v>875</v>
       </c>
       <c r="D454" s="0" t="s">
         <v>58</v>
@@ -29793,13 +29903,13 @@
         <v>488</v>
       </c>
       <c r="G454" s="0" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="H454" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I454" s="0" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="M454" s="0" t="n">
         <v>0</v>
@@ -29837,13 +29947,13 @@
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="1" t="s">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="B455" s="0" t="s">
-        <v>878</v>
+        <v>551</v>
       </c>
       <c r="C455" s="0" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="D455" s="0" t="s">
         <v>58</v>
@@ -29852,13 +29962,13 @@
         <v>492</v>
       </c>
       <c r="G455" s="0" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="H455" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I455" s="0" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="M455" s="0" t="n">
         <v>0</v>
@@ -29896,13 +30006,13 @@
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="1" t="s">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="B456" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="C456" s="0" t="s">
         <v>878</v>
-      </c>
-      <c r="C456" s="0" t="s">
-        <v>885</v>
       </c>
       <c r="D456" s="0" t="s">
         <v>58</v>
@@ -29911,13 +30021,13 @@
         <v>492</v>
       </c>
       <c r="G456" s="0" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="H456" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I456" s="0" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="M456" s="0" t="n">
         <v>0</v>
@@ -29955,13 +30065,13 @@
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="1" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="B457" s="0" t="s">
-        <v>887</v>
+        <v>551</v>
       </c>
       <c r="C457" s="0" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="D457" s="0" t="s">
         <v>58</v>
@@ -29970,13 +30080,13 @@
         <v>488</v>
       </c>
       <c r="G457" s="0" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="H457" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I457" s="0" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="M457" s="0" t="n">
         <v>0</v>
@@ -30014,13 +30124,13 @@
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="1" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="B458" s="0" t="s">
-        <v>887</v>
+        <v>551</v>
       </c>
       <c r="C458" s="0" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="D458" s="0" t="s">
         <v>58</v>
@@ -30029,13 +30139,13 @@
         <v>488</v>
       </c>
       <c r="G458" s="0" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="H458" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I458" s="0" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="M458" s="0" t="n">
         <v>0</v>
@@ -30073,13 +30183,13 @@
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="1" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="B459" s="0" t="s">
-        <v>887</v>
+        <v>551</v>
       </c>
       <c r="C459" s="0" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="D459" s="0" t="s">
         <v>58</v>
@@ -30088,13 +30198,13 @@
         <v>492</v>
       </c>
       <c r="G459" s="0" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="H459" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I459" s="0" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="M459" s="0" t="n">
         <v>0</v>
@@ -30132,13 +30242,13 @@
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="1" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="B460" s="0" t="s">
-        <v>887</v>
+        <v>551</v>
       </c>
       <c r="C460" s="0" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="D460" s="0" t="s">
         <v>58</v>
@@ -30147,13 +30257,13 @@
         <v>492</v>
       </c>
       <c r="G460" s="0" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="H460" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I460" s="0" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="M460" s="0" t="n">
         <v>0</v>
@@ -30191,13 +30301,13 @@
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="1" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="B461" s="0" t="s">
-        <v>896</v>
+        <v>486</v>
       </c>
       <c r="C461" s="0" t="s">
-        <v>897</v>
+        <v>888</v>
       </c>
       <c r="D461" s="0" t="s">
         <v>58</v>
@@ -30206,13 +30316,13 @@
         <v>488</v>
       </c>
       <c r="G461" s="0" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="H461" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I461" s="0" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
       <c r="M461" s="0" t="n">
         <v>0</v>
@@ -30250,13 +30360,13 @@
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="1" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="B462" s="0" t="s">
-        <v>896</v>
+        <v>486</v>
       </c>
       <c r="C462" s="0" t="s">
-        <v>900</v>
+        <v>891</v>
       </c>
       <c r="D462" s="0" t="s">
         <v>58</v>
@@ -30265,13 +30375,13 @@
         <v>488</v>
       </c>
       <c r="G462" s="0" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="H462" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I462" s="0" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
       <c r="M462" s="0" t="n">
         <v>0</v>
@@ -30309,13 +30419,13 @@
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="1" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="B463" s="0" t="s">
-        <v>896</v>
+        <v>486</v>
       </c>
       <c r="C463" s="0" t="s">
-        <v>902</v>
+        <v>893</v>
       </c>
       <c r="D463" s="0" t="s">
         <v>58</v>
@@ -30324,13 +30434,13 @@
         <v>492</v>
       </c>
       <c r="G463" s="0" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="H463" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I463" s="0" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
       <c r="M463" s="0" t="n">
         <v>0</v>
@@ -30368,13 +30478,13 @@
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="1" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="B464" s="0" t="s">
-        <v>896</v>
+        <v>486</v>
       </c>
       <c r="C464" s="0" t="s">
-        <v>903</v>
+        <v>894</v>
       </c>
       <c r="D464" s="0" t="s">
         <v>58</v>
@@ -30383,13 +30493,13 @@
         <v>492</v>
       </c>
       <c r="G464" s="0" t="s">
-        <v>898</v>
+        <v>889</v>
       </c>
       <c r="H464" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I464" s="0" t="s">
-        <v>899</v>
+        <v>890</v>
       </c>
       <c r="M464" s="0" t="n">
         <v>0</v>
@@ -30427,13 +30537,13 @@
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="1" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
       <c r="B465" s="0" t="s">
-        <v>704</v>
+        <v>896</v>
       </c>
       <c r="C465" s="0" t="s">
-        <v>705</v>
+        <v>897</v>
       </c>
       <c r="D465" s="0" t="s">
         <v>58</v>
@@ -30442,13 +30552,13 @@
         <v>488</v>
       </c>
       <c r="G465" s="0" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H465" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I465" s="0" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="M465" s="0" t="n">
         <v>0</v>
@@ -30486,13 +30596,13 @@
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="1" t="s">
-        <v>904</v>
+        <v>895</v>
       </c>
       <c r="B466" s="0" t="s">
-        <v>704</v>
+        <v>896</v>
       </c>
       <c r="C466" s="0" t="s">
-        <v>706</v>
+        <v>900</v>
       </c>
       <c r="D466" s="0" t="s">
         <v>58</v>
@@ -30501,13 +30611,13 @@
         <v>488</v>
       </c>
       <c r="G466" s="0" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H466" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I466" s="0" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="M466" s="0" t="n">
         <v>0</v>
@@ -30545,13 +30655,13 @@
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="1" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="B467" s="0" t="s">
-        <v>704</v>
+        <v>896</v>
       </c>
       <c r="C467" s="0" t="s">
-        <v>708</v>
+        <v>902</v>
       </c>
       <c r="D467" s="0" t="s">
         <v>58</v>
@@ -30560,13 +30670,13 @@
         <v>492</v>
       </c>
       <c r="G467" s="0" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H467" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I467" s="0" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="M467" s="0" t="n">
         <v>0</v>
@@ -30604,13 +30714,13 @@
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="1" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="B468" s="0" t="s">
-        <v>704</v>
+        <v>896</v>
       </c>
       <c r="C468" s="0" t="s">
-        <v>709</v>
+        <v>903</v>
       </c>
       <c r="D468" s="0" t="s">
         <v>58</v>
@@ -30619,13 +30729,13 @@
         <v>492</v>
       </c>
       <c r="G468" s="0" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="H468" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I468" s="0" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="M468" s="0" t="n">
         <v>0</v>
@@ -30661,65 +30771,1185 @@
         <v>0</v>
       </c>
     </row>
-    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="1"/>
-    </row>
-    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A568" s="1"/>
-    </row>
-    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A569" s="1"/>
-    </row>
-    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A570" s="1"/>
-    </row>
-    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A571" s="1"/>
-    </row>
-    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A572" s="1"/>
-    </row>
-    <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A573" s="1"/>
-    </row>
-    <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A574" s="1"/>
-    </row>
-    <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A575" s="1"/>
-    </row>
-    <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A576" s="1"/>
-    </row>
-    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A577" s="1"/>
-    </row>
-    <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A578" s="1"/>
-    </row>
-    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A579" s="1"/>
-    </row>
-    <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A580" s="1"/>
-    </row>
-    <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A581" s="1"/>
-    </row>
-    <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A582" s="1"/>
-    </row>
-    <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A583" s="1"/>
-    </row>
-    <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A584" s="1"/>
-    </row>
-    <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A585" s="1"/>
-    </row>
-    <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A586" s="1"/>
+    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="C469" s="0" t="s">
+        <v>905</v>
+      </c>
+      <c r="D469" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E469" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G469" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="H469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I469" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="M469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S469" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR469" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS469" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="C470" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="D470" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E470" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G470" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="H470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I470" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="M470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S470" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR470" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS470" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B471" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="C471" s="0" t="s">
+        <v>910</v>
+      </c>
+      <c r="D471" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E471" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G471" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="H471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I471" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="M471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S471" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR471" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS471" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B472" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="C472" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="D472" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E472" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G472" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="H472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I472" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="M472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S472" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR472" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS472" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B473" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="C473" s="0" t="s">
+        <v>913</v>
+      </c>
+      <c r="D473" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E473" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G473" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="H473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I473" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="M473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S473" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR473" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS473" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="C474" s="0" t="s">
+        <v>916</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E474" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G474" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="H474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I474" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="M474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S474" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR474" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS474" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="C475" s="0" t="s">
+        <v>918</v>
+      </c>
+      <c r="D475" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E475" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G475" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="H475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I475" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="M475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S475" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR475" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS475" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B476" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="C476" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="D476" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E476" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G476" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="H476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I476" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="M476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S476" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR476" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS476" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="C477" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="D477" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E477" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G477" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="H477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I477" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="M477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S477" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR477" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS477" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B478" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="C478" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="D478" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E478" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G478" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="H478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I478" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="M478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S478" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR478" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS478" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="C479" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="D479" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E479" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G479" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="H479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I479" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="M479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S479" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR479" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS479" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="C480" s="0" t="s">
+        <v>927</v>
+      </c>
+      <c r="D480" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E480" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G480" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="H480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I480" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="M480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S480" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR480" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS480" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B481" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="C481" s="0" t="s">
+        <v>930</v>
+      </c>
+      <c r="D481" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E481" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G481" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="H481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I481" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="M481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S481" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR481" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS481" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="C482" s="0" t="s">
+        <v>933</v>
+      </c>
+      <c r="D482" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E482" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G482" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="H482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I482" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="M482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S482" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR482" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS482" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B483" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="C483" s="0" t="s">
+        <v>935</v>
+      </c>
+      <c r="D483" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E483" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G483" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="H483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I483" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="M483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S483" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR483" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS483" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="C484" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="D484" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E484" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G484" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="H484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I484" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="M484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S484" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR484" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS484" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="C485" s="0" t="s">
+        <v>705</v>
+      </c>
+      <c r="D485" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E485" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G485" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="H485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I485" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="M485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S485" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR485" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS485" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B486" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="C486" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="D486" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E486" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="G486" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="H486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I486" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="M486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S486" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR486" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS486" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="B487" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="C487" s="0" t="s">
+        <v>708</v>
+      </c>
+      <c r="D487" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E487" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G487" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="H487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I487" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="M487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S487" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR487" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS487" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="B488" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="C488" s="0" t="s">
+        <v>709</v>
+      </c>
+      <c r="D488" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E488" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="G488" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="H488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I488" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="M488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S488" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR488" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS488" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="1"/>
@@ -32737,6 +33967,24 @@
     <row r="1258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1258" s="1"/>
     </row>
+    <row r="1259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1259" s="1"/>
+    </row>
+    <row r="1260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1260" s="1"/>
+    </row>
+    <row r="1261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1261" s="1"/>
+    </row>
+    <row r="1262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1262" s="1"/>
+    </row>
+    <row r="1263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1263" s="1"/>
+    </row>
+    <row r="1264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1264" s="1"/>
+    </row>
     <row r="1265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1265" s="1"/>
     </row>
@@ -32779,24 +34027,6 @@
     <row r="1278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1278" s="1"/>
     </row>
-    <row r="1279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1279" s="1"/>
-    </row>
-    <row r="1280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1280" s="1"/>
-    </row>
-    <row r="1281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1281" s="1"/>
-    </row>
-    <row r="1282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1282" s="1"/>
-    </row>
-    <row r="1283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1283" s="1"/>
-    </row>
-    <row r="1284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1284" s="1"/>
-    </row>
     <row r="1285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1285" s="1"/>
     </row>
@@ -32833,6 +34063,36 @@
     <row r="1296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1296" s="1"/>
     </row>
+    <row r="1297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1297" s="1"/>
+    </row>
+    <row r="1298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1298" s="1"/>
+    </row>
+    <row r="1299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1299" s="1"/>
+    </row>
+    <row r="1300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1300" s="1"/>
+    </row>
+    <row r="1301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1301" s="1"/>
+    </row>
+    <row r="1302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1302" s="1"/>
+    </row>
+    <row r="1303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1303" s="1"/>
+    </row>
+    <row r="1304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1304" s="1"/>
+    </row>
+    <row r="1305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1305" s="1"/>
+    </row>
+    <row r="1306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1306" s="1"/>
+    </row>
     <row r="1307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1307" s="1"/>
     </row>
@@ -32863,30 +34123,6 @@
     <row r="1316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1316" s="1"/>
     </row>
-    <row r="1317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1317" s="1"/>
-    </row>
-    <row r="1318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1318" s="1"/>
-    </row>
-    <row r="1321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1321" s="1"/>
-    </row>
-    <row r="1322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1322" s="1"/>
-    </row>
-    <row r="1323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1323" s="1"/>
-    </row>
-    <row r="1324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1324" s="1"/>
-    </row>
-    <row r="1325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1325" s="1"/>
-    </row>
-    <row r="1326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1326" s="1"/>
-    </row>
     <row r="1327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1327" s="1"/>
     </row>
@@ -32902,6 +34138,18 @@
     <row r="1331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1331" s="1"/>
     </row>
+    <row r="1332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1332" s="1"/>
+    </row>
+    <row r="1333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1333" s="1"/>
+    </row>
+    <row r="1334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1334" s="1"/>
+    </row>
+    <row r="1335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1335" s="1"/>
+    </row>
     <row r="1336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1336" s="1"/>
     </row>
@@ -32911,12 +34159,6 @@
     <row r="1338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1338" s="1"/>
     </row>
-    <row r="1339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1339" s="1"/>
-    </row>
-    <row r="1340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1340" s="1"/>
-    </row>
     <row r="1341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1341" s="1"/>
     </row>
@@ -32950,18 +34192,6 @@
     <row r="1351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1351" s="1"/>
     </row>
-    <row r="1352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1352" s="1"/>
-    </row>
-    <row r="1353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1353" s="1"/>
-    </row>
-    <row r="1354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1354" s="1"/>
-    </row>
-    <row r="1355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1355" s="1"/>
-    </row>
     <row r="1356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1356" s="1"/>
     </row>
@@ -33159,6 +34389,66 @@
     </row>
     <row r="1421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1421" s="1"/>
+    </row>
+    <row r="1422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1422" s="1"/>
+    </row>
+    <row r="1423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1423" s="1"/>
+    </row>
+    <row r="1424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1424" s="1"/>
+    </row>
+    <row r="1425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1425" s="1"/>
+    </row>
+    <row r="1426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1426" s="1"/>
+    </row>
+    <row r="1427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1427" s="1"/>
+    </row>
+    <row r="1428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1428" s="1"/>
+    </row>
+    <row r="1429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1429" s="1"/>
+    </row>
+    <row r="1430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1430" s="1"/>
+    </row>
+    <row r="1431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1431" s="1"/>
+    </row>
+    <row r="1432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1432" s="1"/>
+    </row>
+    <row r="1433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1433" s="1"/>
+    </row>
+    <row r="1434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1434" s="1"/>
+    </row>
+    <row r="1435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1435" s="1"/>
+    </row>
+    <row r="1436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1436" s="1"/>
+    </row>
+    <row r="1437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1437" s="1"/>
+    </row>
+    <row r="1438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1438" s="1"/>
+    </row>
+    <row r="1439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1439" s="1"/>
+    </row>
+    <row r="1440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1440" s="1"/>
+    </row>
+    <row r="1441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1441" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
absolute urls to non-localizable images
</commit_message>
<xml_diff>
--- a/run/predefined.xlsx
+++ b/run/predefined.xlsx
@@ -181,7 +181,7 @@
     <t xml:space="preserve">Random Basic Weakness</t>
   </si>
   <si>
-    <t xml:space="preserve">card_images/random_basic_weakness.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/card_images/random_basic_weakness.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Player Card</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">+1</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/p1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/p1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">multi_sided</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/p0.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/p0.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m1</t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">-1</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m2</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">-2</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m2.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m2.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m3</t>
@@ -256,7 +256,7 @@
     <t xml:space="preserve">-3</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m3.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m3.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m4</t>
@@ -265,7 +265,7 @@
     <t xml:space="preserve">-4</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m4.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m4.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m5</t>
@@ -274,7 +274,7 @@
     <t xml:space="preserve">-5</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m5.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m5.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m6</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">-6</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m6.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m6.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m7</t>
@@ -292,7 +292,7 @@
     <t xml:space="preserve">-7</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m7.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m7.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_m8</t>
@@ -301,7 +301,7 @@
     <t xml:space="preserve">-8</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/m8.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/m8.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_elder_sign</t>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">Elder Sign</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/elder_sign.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/elder_sign.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_auto_fail</t>
@@ -319,7 +319,7 @@
     <t xml:space="preserve">Auto Fail</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/auto_fail.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/auto_fail.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_cultist</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve">Cultist</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/cultist.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/cultist.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_elder_thing</t>
@@ -337,7 +337,7 @@
     <t xml:space="preserve">Elder Thing</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/elder_thing.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/elder_thing.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_skull</t>
@@ -346,7 +346,7 @@
     <t xml:space="preserve">Skull</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/skull.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/skull.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_tablet</t>
@@ -355,7 +355,7 @@
     <t xml:space="preserve">Tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/tablet.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/tablet.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_bless</t>
@@ -364,7 +364,7 @@
     <t xml:space="preserve">Bless</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/bless.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/bless.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Innsmouth Conspiracy</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">Curse</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/curse.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/curse.webp</t>
   </si>
   <si>
     <t xml:space="preserve">chaos_frost</t>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">Frost</t>
   </si>
   <si>
-    <t xml:space="preserve">chaos_tokens/frost.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/chaos_tokens/frost.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Edge of the Earth Campaign Expansion</t>
@@ -403,7 +403,7 @@
     <t xml:space="preserve">Lead Investigator</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/first_investigator.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/first_investigator.webp</t>
   </si>
   <si>
     <t xml:space="preserve">FirstInvestigatorToken</t>
@@ -415,7 +415,7 @@
     <t xml:space="preserve">1 Resource</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/resource1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/resource1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenResource1</t>
@@ -427,7 +427,7 @@
     <t xml:space="preserve">3 Resources</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/resource3.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/resource3.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenResource3</t>
@@ -439,7 +439,7 @@
     <t xml:space="preserve">5 Resources</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/resource5.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/resource5.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenResource5</t>
@@ -451,7 +451,7 @@
     <t xml:space="preserve">1 Clue</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/clue1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/clue1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenClueDoom1</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">1 Doom</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/doom1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/doom1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">token_clue_doom_3</t>
@@ -469,7 +469,7 @@
     <t xml:space="preserve">3 Clues</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/clue3.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/clue3.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenClueDoom3</t>
@@ -478,7 +478,7 @@
     <t xml:space="preserve">3 Doom</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/doom3.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/doom3.webp</t>
   </si>
   <si>
     <t xml:space="preserve">token_damage_1</t>
@@ -487,13 +487,13 @@
     <t xml:space="preserve">1 Damage</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/damage1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/damage1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenDamage1</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/damage1_flipped.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/damage1_flipped.webp</t>
   </si>
   <si>
     <t xml:space="preserve">token_damage_3</t>
@@ -502,13 +502,13 @@
     <t xml:space="preserve">3 Damage</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/damage3.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/damage3.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenDamage3</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/damage3_flipped.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/damage3_flipped.webp</t>
   </si>
   <si>
     <t xml:space="preserve">token_horror_1</t>
@@ -517,13 +517,13 @@
     <t xml:space="preserve">1 Horror</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/horror1.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/horror1.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenHorror1</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/horror1_flipped.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/horror1_flipped.webp</t>
   </si>
   <si>
     <t xml:space="preserve">token_horror_3</t>
@@ -532,13 +532,13 @@
     <t xml:space="preserve">3 Horror</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/horror3.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/horror3.webp</t>
   </si>
   <si>
     <t xml:space="preserve">StandardTokenHorror3</t>
   </si>
   <si>
-    <t xml:space="preserve">standard_tokens/horror3_flipped.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/standard_tokens/horror3_flipped.webp</t>
   </si>
   <si>
     <t xml:space="preserve">tfa_binoculars</t>
@@ -772,7 +772,7 @@
     <t xml:space="preserve">Tarot Card</t>
   </si>
   <si>
-    <t xml:space="preserve">card_backs/tarot.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/card_backs/tarot.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Fool • 0 (Reversed)</t>
@@ -1108,7 +1108,7 @@
     <t xml:space="preserve">Red Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_red.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_red.webp</t>
   </si>
   <si>
     <t xml:space="preserve">KeyToken</t>
@@ -1117,7 +1117,7 @@
     <t xml:space="preserve">Unknown Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_unknown.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_unknown.webp</t>
   </si>
   <si>
     <t xml:space="preserve">key_blue</t>
@@ -1126,7 +1126,7 @@
     <t xml:space="preserve">Blue Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_blue.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_blue.webp</t>
   </si>
   <si>
     <t xml:space="preserve">key_green</t>
@@ -1135,7 +1135,7 @@
     <t xml:space="preserve">Green Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_green.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_green.webp</t>
   </si>
   <si>
     <t xml:space="preserve">key_yellow</t>
@@ -1144,7 +1144,7 @@
     <t xml:space="preserve">Yellow Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_yellow.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_yellow.webp</t>
   </si>
   <si>
     <t xml:space="preserve">key_purple</t>
@@ -1153,7 +1153,7 @@
     <t xml:space="preserve">Purple Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_purple.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_purple.webp</t>
   </si>
   <si>
     <t xml:space="preserve">key_black</t>
@@ -1162,7 +1162,7 @@
     <t xml:space="preserve">Black Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_black.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_black.webp</t>
   </si>
   <si>
     <t xml:space="preserve">key_white</t>
@@ -1171,7 +1171,7 @@
     <t xml:space="preserve">White Key</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/key_white.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/key_white.webp</t>
   </si>
   <si>
     <t xml:space="preserve">flooded</t>
@@ -1180,7 +1180,7 @@
     <t xml:space="preserve">Partially Flooded</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/flooded_partially.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/flooded_partially.webp</t>
   </si>
   <si>
     <t xml:space="preserve">FloodedToken</t>
@@ -1189,7 +1189,7 @@
     <t xml:space="preserve">Fully Flooded</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/flooded_fully.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/flooded_fully.webp</t>
   </si>
   <si>
     <t xml:space="preserve">seal_first</t>
@@ -1198,7 +1198,7 @@
     <t xml:space="preserve">Dormant First Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_first_dormant.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_first_dormant.webp</t>
   </si>
   <si>
     <t xml:space="preserve">SealToken</t>
@@ -1207,7 +1207,7 @@
     <t xml:space="preserve">Activated First Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_first_activated.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_first_activated.webp</t>
   </si>
   <si>
     <t xml:space="preserve">seal_second</t>
@@ -1216,13 +1216,13 @@
     <t xml:space="preserve">Dormant Second Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_second_dormant.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_second_dormant.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Activated Second Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_second_activated.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_second_activated.webp</t>
   </si>
   <si>
     <t xml:space="preserve">seal_third</t>
@@ -1231,13 +1231,13 @@
     <t xml:space="preserve">Dormant Third Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_third_dormant.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_third_dormant.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Activated Third Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_third_activated.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_third_activated.webp</t>
   </si>
   <si>
     <t xml:space="preserve">seal_fourth</t>
@@ -1246,13 +1246,13 @@
     <t xml:space="preserve">Dormant Fourth Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_fourth_dormant.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_fourth_dormant.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Activated Fourth Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_fourth_activated.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_fourth_activated.webp</t>
   </si>
   <si>
     <t xml:space="preserve">seal_fifth</t>
@@ -1261,13 +1261,13 @@
     <t xml:space="preserve">Dormant Fifth Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_fifth_dormant.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_fifth_dormant.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Activated Fifth Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">tokens/seal_fifth_activated.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/tokens/seal_fifth_activated.webp</t>
   </si>
   <si>
     <t xml:space="preserve">upg09021</t>
@@ -1717,25 +1717,25 @@
     <t xml:space="preserve">Roland Banks</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/01001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">MiniInvestigator</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/01001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u01001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/01001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">MicroInvestigator</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/01001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m01002</t>
@@ -1744,19 +1744,19 @@
     <t xml:space="preserve">Daisy Walker</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/01002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/01002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u01002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/01002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/01002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m01003</t>
@@ -1765,19 +1765,19 @@
     <t xml:space="preserve">"Skids" O'Toole</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/01003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/01003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u01003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/01003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/01003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m01004</t>
@@ -1786,19 +1786,19 @@
     <t xml:space="preserve">Agnes Baker</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/01004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/01004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u01004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/01004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/01004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m01005</t>
@@ -1807,19 +1807,19 @@
     <t xml:space="preserve">Wendy Adams</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/01005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/01005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/01005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u01005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/01005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/01005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/01005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m01501</t>
@@ -1864,7 +1864,7 @@
     <t xml:space="preserve">Zoey Samaras</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/02001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Dunwich Legacy</t>
@@ -1873,16 +1873,16 @@
     <t xml:space="preserve">dwl</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/02001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u02001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/02001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/02001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m02002</t>
@@ -1891,19 +1891,19 @@
     <t xml:space="preserve">Rex Murphy</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/02002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/02002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u02002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/02002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/02002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m02003</t>
@@ -1912,19 +1912,19 @@
     <t xml:space="preserve">Jenny Barnes</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/02003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/02003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u02003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/02003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/02003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m02004</t>
@@ -1933,19 +1933,19 @@
     <t xml:space="preserve">Jim Culver</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/02004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/02004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u02004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/02004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/02004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m02005</t>
@@ -1954,19 +1954,19 @@
     <t xml:space="preserve">"Ashcan" Pete</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/02005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/02005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/02005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u02005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/02005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/02005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/02005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m03001</t>
@@ -1975,7 +1975,7 @@
     <t xml:space="preserve">Mark Harrigan</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Path to Carcosa</t>
@@ -1984,16 +1984,16 @@
     <t xml:space="preserve">ptc</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u03001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/03001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/03001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m03002</t>
@@ -2002,19 +2002,19 @@
     <t xml:space="preserve">Minh Thi Phan</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/03002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u03002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/03002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/03002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m03003</t>
@@ -2023,19 +2023,19 @@
     <t xml:space="preserve">Sefina Rousseau</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/03003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u03003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/03003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/03003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m03004</t>
@@ -2044,19 +2044,19 @@
     <t xml:space="preserve">Akachi Onyele</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/03004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u03004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/03004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/03004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m03005</t>
@@ -2065,19 +2065,19 @@
     <t xml:space="preserve">William Yorick</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/03005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u03005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/03005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/03005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m03006</t>
@@ -2086,19 +2086,19 @@
     <t xml:space="preserve">Lola Hayes</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/03006a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/03006b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03006a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/03006b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u03006</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/03006a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/03006b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03006a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/03006b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">r03006</t>
@@ -2155,19 +2155,19 @@
     <t xml:space="preserve">Leo Anderson</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/04001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/04001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u04001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/04001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/04001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m04002</t>
@@ -2176,19 +2176,19 @@
     <t xml:space="preserve">Ursula Downs</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/04002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/04002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u04002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/04002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/04002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m04003</t>
@@ -2197,19 +2197,19 @@
     <t xml:space="preserve">Finn Edwards</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/04003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/04003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u04003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/04003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/04003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m04004</t>
@@ -2218,19 +2218,19 @@
     <t xml:space="preserve">Father Mateo</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/04004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/04004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u04004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/04004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/04004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m04005</t>
@@ -2239,19 +2239,19 @@
     <t xml:space="preserve">Calvin Wright</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/04005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/04005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/04005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u04005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/04005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/04005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/04005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05001</t>
@@ -2260,7 +2260,7 @@
     <t xml:space="preserve">Carolyn Fern</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Circle Undone</t>
@@ -2269,16 +2269,16 @@
     <t xml:space="preserve">tcu</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05002</t>
@@ -2287,19 +2287,19 @@
     <t xml:space="preserve">Joe Diamond</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05003</t>
@@ -2308,19 +2308,19 @@
     <t xml:space="preserve">Preston Fairmont</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05004</t>
@@ -2329,19 +2329,19 @@
     <t xml:space="preserve">Diana Stanley</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05005</t>
@@ -2350,19 +2350,19 @@
     <t xml:space="preserve">Rita Young</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05006</t>
@@ -2371,19 +2371,19 @@
     <t xml:space="preserve">Marie Lambeau</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05006a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05006b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05006a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05006b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05006</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05006a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05006b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05006a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05006b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05046</t>
@@ -2392,19 +2392,19 @@
     <t xml:space="preserve">Gavriella Mizrah</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05046a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05046b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05046a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05046b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05046</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05046a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05046b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05046a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05046b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05047</t>
@@ -2413,19 +2413,19 @@
     <t xml:space="preserve">Jerome Davids</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05047a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05047b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05047a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05047b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05047</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05047a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05047b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05047a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05047b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05048</t>
@@ -2434,19 +2434,19 @@
     <t xml:space="preserve">Valentino Rivas</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05048a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05048b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05048a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05048b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05048</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05048a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05048b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05048a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05048b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m05049</t>
@@ -2455,19 +2455,19 @@
     <t xml:space="preserve">Penny White</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/05049a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/05049b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05049a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/05049b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u05049</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/05049a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/05049b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05049a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/05049b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m06001</t>
@@ -2476,7 +2476,7 @@
     <t xml:space="preserve">Tommy Muldoon</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/06001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Dream-Eaters</t>
@@ -2485,16 +2485,16 @@
     <t xml:space="preserve">tde</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/06001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u06001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/06001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/06001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m06002</t>
@@ -2503,19 +2503,19 @@
     <t xml:space="preserve">Mandy Thompson</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/06002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/06002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u06002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/06002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/06002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m06003</t>
@@ -2524,19 +2524,19 @@
     <t xml:space="preserve">Tony Morgan</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/06003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/06003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u06003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/06003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/06003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m06004</t>
@@ -2545,19 +2545,19 @@
     <t xml:space="preserve">Luke Robinson</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/06004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/06004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u06004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/06004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/06004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m06005</t>
@@ -2566,19 +2566,19 @@
     <t xml:space="preserve">Patrice Hathaway</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/06005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/06005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/06005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u06005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/06005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/06005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/06005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m07001</t>
@@ -2587,19 +2587,19 @@
     <t xml:space="preserve">Sister Mary</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/07001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/07001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u07001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/07001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/07001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m07002</t>
@@ -2608,19 +2608,19 @@
     <t xml:space="preserve">Amanda Sharpe</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/07002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/07002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u07002</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/07002a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/07002b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07002a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07002b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m07003</t>
@@ -2629,19 +2629,19 @@
     <t xml:space="preserve">Trish Scarborough</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/07003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/07003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u07003</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/07003a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/07003b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07003a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07003b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m07004</t>
@@ -2650,19 +2650,19 @@
     <t xml:space="preserve">Dexter Drake</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/07004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/07004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u07004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/07004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/07004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m07005</t>
@@ -2671,19 +2671,19 @@
     <t xml:space="preserve">Silas Marsh</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/07005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/07005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/07005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u07005</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/07005a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/07005b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07005a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/07005b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m08001</t>
@@ -2692,7 +2692,7 @@
     <t xml:space="preserve">Daniela Reyes</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/08001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Edge of the Earth Investigator Expansion</t>
@@ -2701,16 +2701,16 @@
     <t xml:space="preserve">eoep</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/08001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u08001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/08001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/08001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m08004</t>
@@ -2719,19 +2719,19 @@
     <t xml:space="preserve">Norman Withers</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/08004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/08004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u08004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/08004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/08004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m08007</t>
@@ -2740,19 +2740,19 @@
     <t xml:space="preserve">Monterey Jack</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/08007a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/08007b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08007a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08007b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u08007</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/08007a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/08007b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08007a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08007b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m08010</t>
@@ -2761,19 +2761,19 @@
     <t xml:space="preserve">Lily Chen</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/08010a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/08010b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08010a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08010b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u08010</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/08010a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/08010b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08010a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08010b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m08016</t>
@@ -2782,19 +2782,19 @@
     <t xml:space="preserve">Bob Jenkins</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/08016a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/08016b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08016a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/08016b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u08016</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/08016a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/08016b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08016a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/08016b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09001</t>
@@ -2803,7 +2803,7 @@
     <t xml:space="preserve">Carson Sinclair</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Scarlet Keys Investigator Expansion</t>
@@ -2812,16 +2812,16 @@
     <t xml:space="preserve">tskp</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/09001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09004</t>
@@ -2830,19 +2830,19 @@
     <t xml:space="preserve">Vincent Lee</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/09004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/09004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09008</t>
@@ -2851,19 +2851,19 @@
     <t xml:space="preserve">Kymani Jones</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09008a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/09008b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09008a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09008b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09008</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09008a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/09008b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09008a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09008b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09011</t>
@@ -2872,19 +2872,19 @@
     <t xml:space="preserve">Amina Zidane</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09011a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/09011b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09011a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09011b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09011</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09011a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/09011b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09011a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09011b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09015</t>
@@ -2893,19 +2893,19 @@
     <t xml:space="preserve">Darrell Simmons</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09015a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/09015b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09015a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09015b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09015</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09015a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/09015b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09015a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09015b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09018</t>
@@ -2914,19 +2914,19 @@
     <t xml:space="preserve">Charlie Kane</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09018a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/09018b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09018a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09018b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09018</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09018a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/09018b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09018a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09018b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m09080</t>
@@ -2935,25 +2935,25 @@
     <t xml:space="preserve">Summoned Servitor</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09080a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09080a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">MiniAssistant</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/09080b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/09080b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u09080</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09080a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09080a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">MicroAssistant</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/09080b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/09080b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m10001</t>
@@ -2962,7 +2962,7 @@
     <t xml:space="preserve">Wilson Richards</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/10001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Feast of Hemlock Vale Investigator Expansion</t>
@@ -2971,16 +2971,16 @@
     <t xml:space="preserve">fhvp</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/10001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u10001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/10001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/10001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m10004</t>
@@ -2989,19 +2989,19 @@
     <t xml:space="preserve">Kate Winthrop</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/10004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/10004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u10004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/10004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/10004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m10009</t>
@@ -3010,19 +3010,19 @@
     <t xml:space="preserve">Alessandra Zorzi</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/10009a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/10009b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10009a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10009b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u10009</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/10009a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/10009b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10009a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10009b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m10012</t>
@@ -3031,19 +3031,19 @@
     <t xml:space="preserve">Kōhaku Narukami</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/10012a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/10012b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10012a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10012b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u10012</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/10012a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/10012b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10012a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10012b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m10015</t>
@@ -3052,19 +3052,19 @@
     <t xml:space="preserve">Hank Samson</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/10015a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/10015b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10015a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/10015b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u10015</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/10015a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/10015b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10015a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/10015b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11001</t>
@@ -3073,7 +3073,7 @@
     <t xml:space="preserve">Marion Tavares</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Drowned City Investigator Expansion</t>
@@ -3082,16 +3082,16 @@
     <t xml:space="preserve">tdcp</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11004</t>
@@ -3100,19 +3100,19 @@
     <t xml:space="preserve">Lucius Galloway</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11007</t>
@@ -3121,37 +3121,37 @@
     <t xml:space="preserve">Agatha Crane</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11007a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11007b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11007a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11007b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11007</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11007a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11007b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11007a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11007b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11008</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11008a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11008b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11008a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11008b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11008</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11008a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11008b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11008a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11008b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11011</t>
@@ -3160,19 +3160,19 @@
     <t xml:space="preserve">Michael McGlen</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11011a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11011b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11011a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11011b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11011</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11011a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11011b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11011a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11011b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11014</t>
@@ -3181,19 +3181,19 @@
     <t xml:space="preserve">Gloria Goldberg</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11014a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11014b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11014a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11014b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11014</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11014a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11014b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11014a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11014b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11017</t>
@@ -3202,19 +3202,19 @@
     <t xml:space="preserve">George Barnaby</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11017a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11017b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11017a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11017b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11017</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11017a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11017b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11017a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11017b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m11068a</t>
@@ -3223,19 +3223,19 @@
     <t xml:space="preserve">Lost Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/11068aa.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mini_investigators/11068ab.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11068aa.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/11068ab.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u11068a</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/11068aa.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/11068ab.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11068aa.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/11068ab.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m60101</t>
@@ -3244,22 +3244,22 @@
     <t xml:space="preserve">Nathaniel Cho</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60101a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60101a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">nat</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60101b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60101b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u60101</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/60101a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/60101b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60101a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60101b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m60201</t>
@@ -3268,22 +3268,22 @@
     <t xml:space="preserve">Harvey Walters</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60201a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60201a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">har</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60201b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60201b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u60201</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/60201a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/60201b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60201a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60201b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m60301</t>
@@ -3292,22 +3292,22 @@
     <t xml:space="preserve">Winifred Habbamock</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60301a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60301a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">win</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60301b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60301b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u60301</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/60301a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/60301b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60301a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60301b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m60401</t>
@@ -3316,22 +3316,22 @@
     <t xml:space="preserve">Jacqueline Fine</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60401a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60401a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">jac</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60401b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60401b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u60401</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/60401a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/60401b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60401a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60401b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m60501</t>
@@ -3340,22 +3340,22 @@
     <t xml:space="preserve">Stella Clark</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60501a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60501a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">ste</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/60501b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/60501b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u60501</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/60501a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/60501b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60501a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/60501b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m89001</t>
@@ -3364,7 +3364,7 @@
     <t xml:space="preserve">Subject 5U-21</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/89001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/89001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Blob That Ate Everything ELSE!</t>
@@ -3373,22 +3373,22 @@
     <t xml:space="preserve">blbe</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/89001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/89001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u89001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/89001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/89001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/89001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/89001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m90084</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/90084a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/90084a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Pistols and Pearls</t>
@@ -3397,22 +3397,22 @@
     <t xml:space="preserve">pap</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/90084b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/90084b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u90084</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/90084a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/90084b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/90084a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/90084b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98001</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98001a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98001a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Hour of the Huntress</t>
@@ -3421,22 +3421,22 @@
     <t xml:space="preserve">hoth</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98001</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98001a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98001b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98001a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98001b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98004</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98004a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98004a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Dirge of Reason</t>
@@ -3445,22 +3445,22 @@
     <t xml:space="preserve">tdor</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98004</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98004a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98004b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98004a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98004b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98007</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98007a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98007a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Ire of the Void</t>
@@ -3469,22 +3469,22 @@
     <t xml:space="preserve">iotv</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98007b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98007b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98007</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98007a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98007b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98007a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98007b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98010</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98010a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98010a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">To Fight the Black Wind</t>
@@ -3493,22 +3493,22 @@
     <t xml:space="preserve">tftbw</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98010b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98010b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98010</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98010a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98010b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98010a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98010b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98013</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98013a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98013a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">The Deep Gate</t>
@@ -3517,22 +3517,22 @@
     <t xml:space="preserve">tdg</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98013b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98013b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98013</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98013a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98013b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98013a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98013b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98016</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98016a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98016a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Blood of Baalshandor</t>
@@ -3541,22 +3541,22 @@
     <t xml:space="preserve">bob</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98016b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98016b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98016</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98016a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98016b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98016a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98016b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m98019</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98019a.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98019a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">Dark Revelations</t>
@@ -3565,16 +3565,16 @@
     <t xml:space="preserve">dre</t>
   </si>
   <si>
-    <t xml:space="preserve">mini_investigators/98019b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/mini_investigators/98019b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">u98019</t>
   </si>
   <si>
-    <t xml:space="preserve">micro_investigators/98019a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">micro_investigators/98019b.webp</t>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98019a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dragncards-ahlcg.s3.amazonaws.com/images/micro_investigators/98019b.webp</t>
   </si>
   <si>
     <t xml:space="preserve">m99001</t>
@@ -3597,7 +3597,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3618,6 +3618,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3662,7 +3669,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3679,6 +3686,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3688,6 +3699,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -3804,17 +3875,17 @@
   </sheetPr>
   <dimension ref="A1:AY1561"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AP1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AP1" activeCellId="0" sqref="AP1"/>
-      <selection pane="bottomLeft" activeCell="AY220" activeCellId="0" sqref="AY220:AY234"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="80.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.18"/>
@@ -7509,7 +7580,7 @@
       <c r="B61" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="4" t="s">
         <v>175</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -7568,7 +7639,7 @@
       <c r="B62" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="4" t="s">
         <v>175</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -7627,7 +7698,7 @@
       <c r="B63" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="4" t="s">
         <v>181</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -7686,7 +7757,7 @@
       <c r="B64" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="4" t="s">
         <v>181</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -7745,7 +7816,7 @@
       <c r="B65" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="4" t="s">
         <v>184</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -7804,7 +7875,7 @@
       <c r="B66" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="4" t="s">
         <v>184</v>
       </c>
       <c r="D66" s="1" t="s">
@@ -7863,7 +7934,7 @@
       <c r="B67" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="4" t="s">
         <v>187</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -7922,7 +7993,7 @@
       <c r="B68" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="4" t="s">
         <v>187</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -7981,7 +8052,7 @@
       <c r="B69" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="4" t="s">
         <v>190</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -8040,7 +8111,7 @@
       <c r="B70" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="4" t="s">
         <v>190</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -8099,7 +8170,7 @@
       <c r="B71" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="4" t="s">
         <v>193</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -8158,7 +8229,7 @@
       <c r="B72" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="4" t="s">
         <v>193</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -8217,7 +8288,7 @@
       <c r="B73" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="4" t="s">
         <v>196</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -8276,7 +8347,7 @@
       <c r="B74" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="4" t="s">
         <v>196</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -8335,7 +8406,7 @@
       <c r="B75" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="4" t="s">
         <v>199</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -8394,7 +8465,7 @@
       <c r="B76" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="4" t="s">
         <v>199</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -8453,7 +8524,7 @@
       <c r="B77" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -8512,7 +8583,7 @@
       <c r="B78" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="4" t="s">
         <v>202</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -8571,7 +8642,7 @@
       <c r="B79" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="4" t="s">
         <v>205</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -8630,7 +8701,7 @@
       <c r="B80" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="4" t="s">
         <v>205</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -8689,7 +8760,7 @@
       <c r="B81" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="4" t="s">
         <v>208</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -8748,7 +8819,7 @@
       <c r="B82" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="4" t="s">
         <v>208</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -8807,7 +8878,7 @@
       <c r="B83" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="4" t="s">
         <v>211</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -8866,7 +8937,7 @@
       <c r="B84" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="4" t="s">
         <v>211</v>
       </c>
       <c r="D84" s="1" t="s">
@@ -8925,7 +8996,7 @@
       <c r="B85" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="4" t="s">
         <v>214</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -8984,7 +9055,7 @@
       <c r="B86" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="4" t="s">
         <v>214</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -9043,7 +9114,7 @@
       <c r="B87" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="4" t="s">
         <v>217</v>
       </c>
       <c r="D87" s="1" t="s">
@@ -9102,7 +9173,7 @@
       <c r="B88" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="4" t="s">
         <v>217</v>
       </c>
       <c r="D88" s="1" t="s">
@@ -9161,7 +9232,7 @@
       <c r="B89" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="4" t="s">
         <v>220</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -9220,7 +9291,7 @@
       <c r="B90" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="4" t="s">
         <v>220</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -9279,7 +9350,7 @@
       <c r="B91" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -9338,7 +9409,7 @@
       <c r="B92" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -9397,7 +9468,7 @@
       <c r="B93" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="4" t="s">
         <v>228</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -9456,7 +9527,7 @@
       <c r="B94" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="4" t="s">
         <v>228</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -9515,7 +9586,7 @@
       <c r="B95" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="4" t="s">
         <v>230</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -9574,7 +9645,7 @@
       <c r="B96" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="4" t="s">
         <v>230</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -9633,7 +9704,7 @@
       <c r="B97" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -9692,7 +9763,7 @@
       <c r="B98" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="4" t="s">
         <v>234</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -9751,7 +9822,7 @@
       <c r="B99" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="4" t="s">
         <v>237</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -9810,7 +9881,7 @@
       <c r="B100" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="4" t="s">
         <v>237</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -9869,7 +9940,7 @@
       <c r="B101" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="4" t="s">
         <v>240</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -9928,7 +9999,7 @@
       <c r="B102" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="4" t="s">
         <v>240</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -9987,7 +10058,7 @@
       <c r="B103" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="4" t="s">
         <v>242</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -10046,7 +10117,7 @@
       <c r="B104" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="4" t="s">
         <v>242</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -10105,7 +10176,7 @@
       <c r="B105" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="4" t="s">
         <v>245</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -10223,7 +10294,7 @@
       <c r="B107" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="4" t="s">
         <v>252</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -10341,7 +10412,7 @@
       <c r="B109" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="4" t="s">
         <v>257</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -10459,7 +10530,7 @@
       <c r="B111" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="4" t="s">
         <v>259</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -10577,7 +10648,7 @@
       <c r="B113" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="4" t="s">
         <v>262</v>
       </c>
       <c r="D113" s="1" t="s">
@@ -10695,7 +10766,7 @@
       <c r="B115" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="4" t="s">
         <v>264</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -10813,7 +10884,7 @@
       <c r="B117" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="4" t="s">
         <v>267</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -10931,7 +11002,7 @@
       <c r="B119" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="4" t="s">
         <v>269</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -11049,7 +11120,7 @@
       <c r="B121" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="4" t="s">
         <v>272</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -11167,7 +11238,7 @@
       <c r="B123" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="4" t="s">
         <v>274</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -11285,7 +11356,7 @@
       <c r="B125" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="4" t="s">
         <v>277</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -11403,7 +11474,7 @@
       <c r="B127" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="4" t="s">
         <v>279</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -11521,7 +11592,7 @@
       <c r="B129" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="4" t="s">
         <v>282</v>
       </c>
       <c r="D129" s="1" t="s">
@@ -11639,7 +11710,7 @@
       <c r="B131" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="4" t="s">
         <v>284</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -11757,7 +11828,7 @@
       <c r="B133" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="4" t="s">
         <v>287</v>
       </c>
       <c r="D133" s="1" t="s">
@@ -11875,7 +11946,7 @@
       <c r="B135" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" s="4" t="s">
         <v>289</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -11993,7 +12064,7 @@
       <c r="B137" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C137" s="4" t="s">
         <v>292</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -12111,7 +12182,7 @@
       <c r="B139" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C139" s="4" t="s">
         <v>294</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -12229,7 +12300,7 @@
       <c r="B141" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" s="4" t="s">
         <v>297</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -12347,7 +12418,7 @@
       <c r="B143" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C143" s="4" t="s">
         <v>299</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -12465,7 +12536,7 @@
       <c r="B145" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C145" s="4" t="s">
         <v>302</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -12583,7 +12654,7 @@
       <c r="B147" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C147" s="4" t="s">
         <v>304</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -12701,7 +12772,7 @@
       <c r="B149" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="4" t="s">
         <v>307</v>
       </c>
       <c r="D149" s="1" t="s">
@@ -12819,7 +12890,7 @@
       <c r="B151" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C151" s="4" t="s">
         <v>309</v>
       </c>
       <c r="D151" s="1" t="s">
@@ -12937,7 +13008,7 @@
       <c r="B153" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" s="4" t="s">
         <v>312</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -13055,7 +13126,7 @@
       <c r="B155" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C155" s="1" t="s">
+      <c r="C155" s="4" t="s">
         <v>314</v>
       </c>
       <c r="D155" s="1" t="s">
@@ -13173,7 +13244,7 @@
       <c r="B157" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C157" s="1" t="s">
+      <c r="C157" s="4" t="s">
         <v>317</v>
       </c>
       <c r="D157" s="1" t="s">
@@ -13291,7 +13362,7 @@
       <c r="B159" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C159" s="1" t="s">
+      <c r="C159" s="4" t="s">
         <v>319</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -13409,7 +13480,7 @@
       <c r="B161" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C161" s="1" t="s">
+      <c r="C161" s="4" t="s">
         <v>322</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -13527,7 +13598,7 @@
       <c r="B163" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C163" s="1" t="s">
+      <c r="C163" s="4" t="s">
         <v>324</v>
       </c>
       <c r="D163" s="1" t="s">
@@ -13645,7 +13716,7 @@
       <c r="B165" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C165" s="1" t="s">
+      <c r="C165" s="4" t="s">
         <v>327</v>
       </c>
       <c r="D165" s="1" t="s">
@@ -13763,7 +13834,7 @@
       <c r="B167" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C167" s="4" t="s">
         <v>329</v>
       </c>
       <c r="D167" s="1" t="s">
@@ -13881,7 +13952,7 @@
       <c r="B169" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C169" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D169" s="1" t="s">
@@ -13999,7 +14070,7 @@
       <c r="B171" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C171" s="1" t="s">
+      <c r="C171" s="4" t="s">
         <v>334</v>
       </c>
       <c r="D171" s="1" t="s">
@@ -14117,7 +14188,7 @@
       <c r="B173" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C173" s="1" t="s">
+      <c r="C173" s="4" t="s">
         <v>337</v>
       </c>
       <c r="D173" s="1" t="s">
@@ -14235,7 +14306,7 @@
       <c r="B175" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C175" s="4" t="s">
         <v>339</v>
       </c>
       <c r="D175" s="1" t="s">
@@ -14353,7 +14424,7 @@
       <c r="B177" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="C177" s="4" t="s">
         <v>342</v>
       </c>
       <c r="D177" s="1" t="s">
@@ -14471,7 +14542,7 @@
       <c r="B179" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C179" s="1" t="s">
+      <c r="C179" s="4" t="s">
         <v>344</v>
       </c>
       <c r="D179" s="1" t="s">
@@ -14589,7 +14660,7 @@
       <c r="B181" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C181" s="4" t="s">
         <v>347</v>
       </c>
       <c r="D181" s="1" t="s">
@@ -14707,7 +14778,7 @@
       <c r="B183" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C183" s="4" t="s">
         <v>349</v>
       </c>
       <c r="D183" s="1" t="s">
@@ -14825,7 +14896,7 @@
       <c r="B185" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C185" s="1" t="s">
+      <c r="C185" s="4" t="s">
         <v>352</v>
       </c>
       <c r="D185" s="1" t="s">
@@ -14943,7 +15014,7 @@
       <c r="B187" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="C187" s="4" t="s">
         <v>354</v>
       </c>
       <c r="D187" s="1" t="s">
@@ -15061,7 +15132,7 @@
       <c r="B189" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C189" s="1" t="s">
+      <c r="C189" s="4" t="s">
         <v>357</v>
       </c>
       <c r="D189" s="1" t="s">
@@ -15179,7 +15250,7 @@
       <c r="B191" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C191" s="1" t="s">
+      <c r="C191" s="4" t="s">
         <v>359</v>
       </c>
       <c r="D191" s="1" t="s">
@@ -16831,7 +16902,7 @@
       <c r="B219" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="C219" s="1" t="s">
+      <c r="C219" s="4" t="s">
         <v>418</v>
       </c>
       <c r="D219" s="1" t="s">
@@ -16887,7 +16958,7 @@
       <c r="B220" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C220" s="1" t="s">
+      <c r="C220" s="4" t="s">
         <v>425</v>
       </c>
       <c r="D220" s="1" t="s">
@@ -16943,7 +17014,7 @@
       <c r="B221" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C221" s="1" t="s">
+      <c r="C221" s="4" t="s">
         <v>427</v>
       </c>
       <c r="D221" s="1" t="s">
@@ -17008,7 +17079,7 @@
       <c r="B222" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="4" t="s">
         <v>431</v>
       </c>
       <c r="D222" s="1" t="s">
@@ -17064,7 +17135,7 @@
       <c r="B223" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C223" s="2" t="s">
+      <c r="C223" s="4" t="s">
         <v>434</v>
       </c>
       <c r="D223" s="1" t="s">
@@ -17120,7 +17191,7 @@
       <c r="B224" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="C224" s="4" t="s">
         <v>437</v>
       </c>
       <c r="D224" s="1" t="s">
@@ -17176,7 +17247,7 @@
       <c r="B225" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C225" s="2" t="s">
+      <c r="C225" s="4" t="s">
         <v>437</v>
       </c>
       <c r="D225" s="1" t="s">
@@ -17241,7 +17312,7 @@
       <c r="B226" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="C226" s="4" t="s">
         <v>442</v>
       </c>
       <c r="D226" s="1" t="s">
@@ -17297,7 +17368,7 @@
       <c r="B227" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C227" s="2" t="s">
+      <c r="C227" s="4" t="s">
         <v>445</v>
       </c>
       <c r="D227" s="1" t="s">
@@ -17353,7 +17424,7 @@
       <c r="B228" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="C228" s="4" t="s">
         <v>448</v>
       </c>
       <c r="D228" s="1" t="s">
@@ -17409,7 +17480,7 @@
       <c r="B229" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C229" s="2" t="s">
+      <c r="C229" s="4" t="s">
         <v>451</v>
       </c>
       <c r="D229" s="1" t="s">
@@ -17465,7 +17536,7 @@
       <c r="B230" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="C230" s="2" t="s">
+      <c r="C230" s="4" t="s">
         <v>454</v>
       </c>
       <c r="D230" s="1" t="s">
@@ -17521,7 +17592,7 @@
       <c r="B231" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C231" s="2" t="s">
+      <c r="C231" s="4" t="s">
         <v>457</v>
       </c>
       <c r="D231" s="1" t="s">
@@ -17577,7 +17648,7 @@
       <c r="B232" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="C232" s="4" t="s">
         <v>460</v>
       </c>
       <c r="D232" s="1" t="s">
@@ -17633,7 +17704,7 @@
       <c r="B233" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C233" s="4" t="s">
         <v>462</v>
       </c>
       <c r="D233" s="1" t="s">
@@ -17698,7 +17769,7 @@
       <c r="B234" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C234" s="2" t="s">
+      <c r="C234" s="4" t="s">
         <v>462</v>
       </c>
       <c r="D234" s="1" t="s">
@@ -17763,7 +17834,7 @@
       <c r="B235" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C235" s="2" t="s">
+      <c r="C235" s="4" t="s">
         <v>467</v>
       </c>
       <c r="D235" s="1" t="s">
@@ -17819,7 +17890,7 @@
       <c r="B236" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C236" s="2" t="s">
+      <c r="C236" s="4" t="s">
         <v>470</v>
       </c>
       <c r="D236" s="1" t="s">
@@ -17875,7 +17946,7 @@
       <c r="B237" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="C237" s="2" t="s">
+      <c r="C237" s="4" t="s">
         <v>473</v>
       </c>
       <c r="D237" s="1" t="s">
@@ -17931,7 +18002,7 @@
       <c r="B238" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C238" s="2" t="s">
+      <c r="C238" s="4" t="s">
         <v>476</v>
       </c>
       <c r="D238" s="1" t="s">
@@ -17987,7 +18058,7 @@
       <c r="B239" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="C239" s="1" t="s">
+      <c r="C239" s="4" t="s">
         <v>479</v>
       </c>
       <c r="D239" s="1" t="s">
@@ -18043,7 +18114,7 @@
       <c r="B240" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="C240" s="1" t="s">
+      <c r="C240" s="4" t="s">
         <v>484</v>
       </c>
       <c r="D240" s="1" t="s">
@@ -18099,7 +18170,7 @@
       <c r="B241" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C241" s="1" t="s">
+      <c r="C241" s="4" t="s">
         <v>487</v>
       </c>
       <c r="D241" s="1" t="s">
@@ -18155,7 +18226,7 @@
       <c r="B242" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="C242" s="1" t="s">
+      <c r="C242" s="4" t="s">
         <v>490</v>
       </c>
       <c r="D242" s="1" t="s">
@@ -18211,7 +18282,7 @@
       <c r="B243" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C243" s="1" t="s">
+      <c r="C243" s="4" t="s">
         <v>493</v>
       </c>
       <c r="D243" s="1" t="s">
@@ -18267,7 +18338,7 @@
       <c r="B244" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="C244" s="1" t="s">
+      <c r="C244" s="4" t="s">
         <v>496</v>
       </c>
       <c r="D244" s="1" t="s">
@@ -18323,7 +18394,7 @@
       <c r="B245" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C245" s="1" t="s">
+      <c r="C245" s="4" t="s">
         <v>499</v>
       </c>
       <c r="D245" s="1" t="s">
@@ -18379,7 +18450,7 @@
       <c r="B246" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C246" s="1" t="s">
+      <c r="C246" s="4" t="s">
         <v>502</v>
       </c>
       <c r="D246" s="1" t="s">
@@ -18435,7 +18506,7 @@
       <c r="B247" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="C247" s="1" t="s">
+      <c r="C247" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D247" s="1" t="s">
@@ -18491,7 +18562,7 @@
       <c r="B248" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="C248" s="1" t="s">
+      <c r="C248" s="4" t="s">
         <v>508</v>
       </c>
       <c r="D248" s="1" t="s">
@@ -18547,7 +18618,7 @@
       <c r="B249" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C249" s="1" t="s">
+      <c r="C249" s="4" t="s">
         <v>511</v>
       </c>
       <c r="D249" s="1" t="s">
@@ -18603,7 +18674,7 @@
       <c r="B250" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C250" s="1" t="s">
+      <c r="C250" s="4" t="s">
         <v>514</v>
       </c>
       <c r="D250" s="1" t="s">
@@ -18659,7 +18730,7 @@
       <c r="B251" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C251" s="1" t="s">
+      <c r="C251" s="4" t="s">
         <v>517</v>
       </c>
       <c r="D251" s="1" t="s">
@@ -18715,7 +18786,7 @@
       <c r="B252" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="C252" s="1" t="s">
+      <c r="C252" s="4" t="s">
         <v>520</v>
       </c>
       <c r="D252" s="1" t="s">
@@ -18771,7 +18842,7 @@
       <c r="B253" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="C253" s="1" t="s">
+      <c r="C253" s="4" t="s">
         <v>523</v>
       </c>
       <c r="D253" s="1" t="s">
@@ -18827,7 +18898,7 @@
       <c r="B254" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="C254" s="1" t="s">
+      <c r="C254" s="4" t="s">
         <v>526</v>
       </c>
       <c r="D254" s="1" t="s">
@@ -18883,7 +18954,7 @@
       <c r="B255" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="C255" s="1" t="s">
+      <c r="C255" s="4" t="s">
         <v>529</v>
       </c>
       <c r="D255" s="1" t="s">
@@ -18939,7 +19010,7 @@
       <c r="B256" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="C256" s="1" t="s">
+      <c r="C256" s="4" t="s">
         <v>532</v>
       </c>
       <c r="D256" s="1" t="s">
@@ -18995,7 +19066,7 @@
       <c r="B257" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C257" s="1" t="s">
+      <c r="C257" s="4" t="s">
         <v>535</v>
       </c>
       <c r="D257" s="1" t="s">
@@ -19051,7 +19122,7 @@
       <c r="B258" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="C258" s="1" t="s">
+      <c r="C258" s="4" t="s">
         <v>538</v>
       </c>
       <c r="D258" s="1" t="s">
@@ -19107,7 +19178,7 @@
       <c r="B259" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="C259" s="1" t="s">
+      <c r="C259" s="4" t="s">
         <v>541</v>
       </c>
       <c r="D259" s="1" t="s">
@@ -19163,7 +19234,7 @@
       <c r="B260" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="C260" s="1" t="s">
+      <c r="C260" s="4" t="s">
         <v>544</v>
       </c>
       <c r="D260" s="1" t="s">
@@ -19219,7 +19290,7 @@
       <c r="B261" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="C261" s="1" t="s">
+      <c r="C261" s="4" t="s">
         <v>547</v>
       </c>
       <c r="D261" s="1" t="s">
@@ -19275,7 +19346,7 @@
       <c r="B262" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C262" s="1" t="s">
+      <c r="C262" s="4" t="s">
         <v>550</v>
       </c>
       <c r="D262" s="1" t="s">
@@ -19331,7 +19402,7 @@
       <c r="B263" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="C263" s="1" t="s">
+      <c r="C263" s="4" t="s">
         <v>553</v>
       </c>
       <c r="D263" s="1" t="s">
@@ -19387,7 +19458,7 @@
       <c r="B264" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="C264" s="1" t="s">
+      <c r="C264" s="4" t="s">
         <v>556</v>
       </c>
       <c r="D264" s="1" t="s">
@@ -19443,7 +19514,7 @@
       <c r="B265" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C265" s="1" t="s">
+      <c r="C265" s="4" t="s">
         <v>559</v>
       </c>
       <c r="D265" s="1" t="s">
@@ -19499,7 +19570,7 @@
       <c r="B266" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="C266" s="1" t="s">
+      <c r="C266" s="4" t="s">
         <v>562</v>
       </c>
       <c r="D266" s="1" t="s">
@@ -24511,7 +24582,7 @@
       <c r="B351" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="C351" s="1" t="s">
+      <c r="C351" s="4" t="s">
         <v>695</v>
       </c>
       <c r="D351" s="1" t="s">
@@ -24570,7 +24641,7 @@
       <c r="B352" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="C352" s="1" t="s">
+      <c r="C352" s="4" t="s">
         <v>698</v>
       </c>
       <c r="D352" s="1" t="s">
@@ -24629,7 +24700,7 @@
       <c r="B353" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="C353" s="1" t="s">
+      <c r="C353" s="4" t="s">
         <v>700</v>
       </c>
       <c r="D353" s="1" t="s">
@@ -24688,7 +24759,7 @@
       <c r="B354" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="C354" s="1" t="s">
+      <c r="C354" s="4" t="s">
         <v>702</v>
       </c>
       <c r="D354" s="1" t="s">
@@ -24747,7 +24818,7 @@
       <c r="B355" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="C355" s="1" t="s">
+      <c r="C355" s="4" t="s">
         <v>704</v>
       </c>
       <c r="D355" s="1" t="s">
@@ -24806,7 +24877,7 @@
       <c r="B356" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="C356" s="1" t="s">
+      <c r="C356" s="4" t="s">
         <v>707</v>
       </c>
       <c r="D356" s="1" t="s">

</xml_diff>